<commit_message>
Atualização da extração de dados
Após extração de Candotti et al., 2023
</commit_message>
<xml_diff>
--- a/Extração dos dados.xlsx
+++ b/Extração dos dados.xlsx
@@ -8,17 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pichau\Documents\ProjetosTese\10-anos-de-back-pei\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD905749-B16C-408B-9DC1-03DA8E524BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{481989D1-0AB2-4B2A-A0AB-025F3C3F8DF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13980" yWindow="0" windowWidth="14985" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -59,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="114">
   <si>
     <t>Autor</t>
   </si>
@@ -706,13 +717,100 @@
   </si>
   <si>
     <t>O BackPEI-CA é uma ferramenta válida e confiável que pode ser utilizada em avaliações clínicas e rasteramento nas escolas.</t>
+  </si>
+  <si>
+    <t>Atualizar o BackPEI-A incluindo 4 novas questões sore o uso de dispositivos móveis. Apresentar um novo design dos aspectos relacionados à dor nas costas e pescoço para facilitar a compreensão da localização destas dores. Testar a validade de conteúdo e confiabilidade das novas questões. Identificar se a versão online do BackPEI-A possui confiabilidade adequada</t>
+  </si>
+  <si>
+    <t>Revisão de literatura para identificar as posturas adotadas ao utilizar dispositivos móveis</t>
+  </si>
+  <si>
+    <t>Inclusão das novas questões</t>
+  </si>
+  <si>
+    <t>Validade de conteúdo</t>
+  </si>
+  <si>
+    <t>Versão final do BackPEI-A</t>
+  </si>
+  <si>
+    <t>Avaliação da confiabilidade</t>
+  </si>
+  <si>
+    <t>Questões novas: 2 questões sobre as posições ao utilizar celulares; 1 sobre o tempo de uso de dispositivos móveis. Uma questão alterada, aquela sobre ler e/ou estudar na cama foi acrescida do uso de um dispositivo móvel. Ainda foram inseridos desenhos esquemáticos para apoiar as questões relativas a dor nas costas e pescoço</t>
+  </si>
+  <si>
+    <r>
+      <t>8 especialistas / Avaliaram: a clareza, facilidade de compreensão e aplicabilidade das novas questões e novo design; se as novas questões permitem a identificação dos comportamentos de uso de smartphone/tablet / /escala likert de 3 níveis sendo o questionário revisado em avaliações nos níveis inferiores até o consenso / CVI (CVI</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>≥</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>0,8)</t>
+    </r>
+  </si>
+  <si>
+    <t>2 rodadas. Comportamentos com CVI=0,87 e novas questões e design com CVI=1</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">194 indivíduos / Aplicação em um intervalo de 7 dias por 2 grupos: impresso (n=80) e online (n=79) / %C (&gt;50%), </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>κ (&gt;0,4), ICC</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>2,2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, SEM e MDC</t>
+    </r>
+  </si>
+  <si>
+    <t>Todos os valores de %C&gt;50% e κ&gt;0,4. Para a amostra geral o κ médio foi de 0,579 variando de 0,511 a 0,667 e o %C médio de 71,8% variando de 67,1% a 76,1%. Para a versão onlineo κ médio foi de 0,676 variando de 0,465 a 0,946 e o %C médio de 82,0% variando de 60,6% a 97,5%. Intensidade da dor nas costas (ICC=0,595, SEM=1,26, MDC=2,48), Intensidade da dor no pescoço (ICC=0,479, SEM=1,68, MDC=3,10)</t>
+  </si>
+  <si>
+    <t>A atualização do BackPEI-A com seu novo design  e questões sobre o uso de dispositivos móveis é válida e confiável.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -766,6 +864,13 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -823,19 +928,19 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1117,11 +1222,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1129,9 +1234,9 @@
     <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="76" style="2" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="3"/>
-    <col min="5" max="5" width="76" style="4" customWidth="1"/>
+    <col min="5" max="5" width="50.5703125" style="4" customWidth="1"/>
     <col min="6" max="6" width="76" style="5" customWidth="1"/>
-    <col min="7" max="7" width="75.7109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="55.42578125" style="4" customWidth="1"/>
     <col min="8" max="8" width="39.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1162,10 +1267,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="16">
+      <c r="B2" s="14">
         <v>2013</v>
       </c>
       <c r="C2" s="13" t="s">
@@ -1188,8 +1293,8 @@
       </c>
     </row>
     <row r="3" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
       <c r="C3" s="13"/>
       <c r="D3" s="3">
         <v>2</v>
@@ -1205,8 +1310,8 @@
       </c>
     </row>
     <row r="4" spans="1:8" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
       <c r="C4" s="13"/>
       <c r="D4" s="3">
         <v>3</v>
@@ -1222,8 +1327,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
       <c r="C5" s="13"/>
       <c r="D5" s="3">
         <v>4</v>
@@ -1235,8 +1340,8 @@
       <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16"/>
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
       <c r="C6" s="13"/>
       <c r="D6" s="3">
         <v>5</v>
@@ -1248,8 +1353,8 @@
       <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:8" s="3" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
       <c r="C7" s="13"/>
       <c r="D7" s="3">
         <v>6</v>
@@ -1257,7 +1362,7 @@
       <c r="E7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="12" t="s">
         <v>25</v>
       </c>
       <c r="G7" s="4" t="s">
@@ -1265,8 +1370,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
       <c r="C8" s="13"/>
       <c r="D8" s="3">
         <v>7</v>
@@ -1274,12 +1379,12 @@
       <c r="E8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="15"/>
+      <c r="F8" s="12"/>
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:8" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
+      <c r="A9" s="14"/>
+      <c r="B9" s="14"/>
       <c r="C9" s="13"/>
       <c r="D9" s="3">
         <v>8</v>
@@ -1287,14 +1392,14 @@
       <c r="E9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="15"/>
+      <c r="F9" s="12"/>
       <c r="G9" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
       <c r="C10" s="13"/>
       <c r="D10" s="3">
         <v>9</v>
@@ -1308,8 +1413,8 @@
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="16"/>
+      <c r="A11" s="14"/>
+      <c r="B11" s="14"/>
       <c r="C11" s="13"/>
       <c r="D11" s="3">
         <v>10</v>
@@ -1321,8 +1426,8 @@
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:8" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
-      <c r="B12" s="16"/>
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
       <c r="C12" s="13"/>
       <c r="D12" s="3">
         <v>11</v>
@@ -1338,8 +1443,8 @@
       </c>
     </row>
     <row r="13" spans="1:8" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
-      <c r="B13" s="16"/>
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
       <c r="C13" s="13"/>
       <c r="D13" s="3">
         <v>12</v>
@@ -1376,10 +1481,10 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="14">
+      <c r="B15" s="15">
         <v>2018</v>
       </c>
       <c r="C15" s="13" t="s">
@@ -1391,7 +1496,7 @@
       <c r="E15" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="15" t="s">
+      <c r="F15" s="12" t="s">
         <v>46</v>
       </c>
       <c r="G15" s="4" t="s">
@@ -1402,8 +1507,8 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
       <c r="C16" s="13"/>
       <c r="D16" s="3">
         <v>2</v>
@@ -1411,14 +1516,14 @@
       <c r="E16" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F16" s="15"/>
+      <c r="F16" s="12"/>
       <c r="G16" s="4" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
       <c r="C17" s="13"/>
       <c r="D17" s="3">
         <v>3</v>
@@ -1426,14 +1531,14 @@
       <c r="E17" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F17" s="15"/>
+      <c r="F17" s="12"/>
       <c r="G17" s="4" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
+      <c r="A18" s="15"/>
+      <c r="B18" s="15"/>
       <c r="C18" s="13"/>
       <c r="D18" s="3">
         <v>4</v>
@@ -1449,8 +1554,8 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="63" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-      <c r="B19" s="14"/>
+      <c r="A19" s="15"/>
+      <c r="B19" s="15"/>
       <c r="C19" s="13"/>
       <c r="D19" s="3">
         <v>5</v>
@@ -1466,8 +1571,8 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="14"/>
+      <c r="A20" s="15"/>
+      <c r="B20" s="15"/>
       <c r="C20" s="13"/>
       <c r="D20" s="3">
         <v>6</v>
@@ -1480,8 +1585,8 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="14"/>
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
       <c r="C21" s="13"/>
       <c r="E21" s="4" t="s">
         <v>58</v>
@@ -1517,10 +1622,10 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B23" s="14">
+      <c r="B23" s="15">
         <v>2019</v>
       </c>
       <c r="C23" s="13" t="s">
@@ -1540,8 +1645,8 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
-      <c r="B24" s="14"/>
+      <c r="A24" s="15"/>
+      <c r="B24" s="15"/>
       <c r="C24" s="13"/>
       <c r="E24" s="4" t="s">
         <v>66</v>
@@ -1554,8 +1659,8 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
-      <c r="B25" s="14"/>
+      <c r="A25" s="15"/>
+      <c r="B25" s="15"/>
       <c r="C25" s="13"/>
       <c r="E25" s="4" t="s">
         <v>68</v>
@@ -1568,8 +1673,8 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A26" s="14"/>
-      <c r="B26" s="14"/>
+      <c r="A26" s="15"/>
+      <c r="B26" s="15"/>
       <c r="C26" s="13"/>
       <c r="E26" s="4" t="s">
         <v>64</v>
@@ -1582,8 +1687,8 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="14"/>
-      <c r="B27" s="14"/>
+      <c r="A27" s="15"/>
+      <c r="B27" s="15"/>
       <c r="C27" s="13"/>
       <c r="E27" s="4" t="s">
         <v>45</v>
@@ -1596,10 +1701,10 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
+      <c r="A28" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="B28" s="12">
+      <c r="B28" s="16">
         <v>2021</v>
       </c>
       <c r="C28" s="13" t="s">
@@ -1619,8 +1724,8 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
-      <c r="B29" s="12"/>
+      <c r="A29" s="16"/>
+      <c r="B29" s="16"/>
       <c r="C29" s="13"/>
       <c r="E29" s="4" t="s">
         <v>81</v>
@@ -1634,8 +1739,8 @@
       <c r="H29" s="13"/>
     </row>
     <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="12"/>
+      <c r="A30" s="16"/>
+      <c r="B30" s="16"/>
       <c r="C30" s="13"/>
       <c r="E30" s="4" t="s">
         <v>82</v>
@@ -1679,7 +1784,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="5:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="E33" s="4" t="s">
         <v>95</v>
       </c>
@@ -1690,7 +1795,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="34" spans="5:7" ht="96" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="96" x14ac:dyDescent="0.25">
       <c r="E34" s="4" t="s">
         <v>82</v>
       </c>
@@ -1701,7 +1806,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="35" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E35" s="4" t="s">
         <v>16</v>
       </c>
@@ -1709,8 +1814,75 @@
         <v>23</v>
       </c>
     </row>
+    <row r="36" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36">
+        <v>2023</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F36" s="4"/>
+      <c r="H36" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="E37" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="E38" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E39" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="F39" s="4"/>
+    </row>
+    <row r="40" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="E40" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E41" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F41" s="4"/>
+    </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="H28:H30"/>
+    <mergeCell ref="C23:C27"/>
+    <mergeCell ref="B23:B27"/>
+    <mergeCell ref="A23:A27"/>
     <mergeCell ref="F7:F9"/>
     <mergeCell ref="C2:C13"/>
     <mergeCell ref="A2:A13"/>
@@ -1719,13 +1891,6 @@
     <mergeCell ref="C15:C21"/>
     <mergeCell ref="B15:B21"/>
     <mergeCell ref="A15:A21"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="H28:H30"/>
-    <mergeCell ref="C23:C27"/>
-    <mergeCell ref="B23:B27"/>
-    <mergeCell ref="A23:A27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualização de Extração de dados
Após leitura de Bebiş e Gençbaş 2019
</commit_message>
<xml_diff>
--- a/Extração dos dados.xlsx
+++ b/Extração dos dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pichau\Documents\ProjetosTese\10-anos-de-back-pei\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0046901C-4C1B-4138-93FA-62F809ADCAA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB75DD8-C9A8-4F3B-A9CA-46AAA6F38BE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="279">
   <si>
     <t>Autor</t>
   </si>
@@ -877,9 +877,6 @@
     <t>Validade de critério (concorrente)</t>
   </si>
   <si>
-    <t>139 estudantes / Associação entre a intensidade da dor e  / Correlação de Spearman</t>
-  </si>
-  <si>
     <t>139 estudantes / KMO (&lt;0,5) e teste de esfericidade de Bartlett (p&gt;0,05)</t>
   </si>
   <si>
@@ -1324,6 +1321,54 @@
   </si>
   <si>
     <t>pode ser aplicável a qualquer ambiente profissional específico onde dores nas costas e no pescoço sejam o foco da prática.</t>
+  </si>
+  <si>
+    <t>O risco de desenvolver dor nas costas durante a adolescência é atribuído a causas multifatoriais, como gênero, idade, atividade física intensa, tabagismo, ansiedade e depressão, além da presença de lombalgia na família (1). No entanto, fatores ambientais nas escolas também influenciam significativamente a dor nas costas durante esse período. Esses fatores incluem estilos de vida sedentários na escola, períodos prolongados sentados, uso excessivo de computadores, hábitos de carregar bolsas pesadas e inadequadas, distúrbios posturais típicos dessa idade e deformidades da coluna vertebral, como cifose, escoliose ou escápula alada, que podem se desenvolver nessa idade. Além disso, a falta de condições ergonômicas nas carteiras e cadeiras escolares desempenha um papel importante na dor nas costas em adolescentes.</t>
+  </si>
+  <si>
+    <t>Bebiş e Gençbaş 2019</t>
+  </si>
+  <si>
+    <t>Além de ferramentas que fornecem dados quantitativos para medir problemas como questões posturais e sintomas de dor nas costas em adolescentes, raramente há ferramentas desenvolvidas para obter dados qualitativos.</t>
+  </si>
+  <si>
+    <t>A literature review in Turkey revealed a lack of tools specifically designed to obtain data related to back pain and posture for the adolescent group</t>
+  </si>
+  <si>
+    <t>O Instrumento de Avaliação de Dor nas Costas e Postura Corporal (BackPEI) foi desenvolvido por Noll, Candotti, Vieira e Loss (2012) para avaliar os hábitos comportamentais e posturais de estudantes e a frequência de dor nas costas (12). Este instrumento é composto por seis seções:
+- Dados demográficos (idade e sexo),
+- Nível socioeconômico (questões como nível de escolaridade dos pais),
+- Fatores comportamentais (atividade física, leitura na cama, horas gastas assistindo TV ou usando o computador diariamente, duração do sono diário),
+- Dor nas costas nos últimos três meses (ocorrência, frequência e intensidade),
+- Fatores posturais (postura sentada ao usar o computador ou escrever, postura sentada em sala de aula, método de transporte de materiais escolares, posição para dormir),
+- Fatores genéticos (presença de dor nas costas nos pais).</t>
+  </si>
+  <si>
+    <t>139 estudantes / Associação entre a intensidade da dor e presençã da dor / Correlação de Spearman</t>
+  </si>
+  <si>
+    <t>A validade da escala em turco foi assegurada por cinco professores especialistas na área e proficientes em inglês, que a traduziram para o turco. Um professor de língua turca avaliou sua gramática e compreensibilidade em turco.</t>
+  </si>
+  <si>
+    <t>Como a escala não é do tipo Likert, a análise fatorial — normalmente necessária para avaliar a validade de construto — não foi realizada. Em vez disso, a adequação dos dados para a análise fatorial foi examinada usando o coeficiente de Kaiser-Meyer-Olkin (KMO) e o Teste de Esfericidade de Bartlett.</t>
+  </si>
+  <si>
+    <t>No estudo de confiabilidade, foram avaliados o coeficiente alfa de Cronbach, a correlação entre itens totais e o coeficiente de confiabilidade teste-reteste (coeficiente kappa). O teste t foi realizado em grupos dependentes para avaliar os resultados do teste-reteste. Os dados foram avaliados com um intervalo de confiança de 95% e um nível de significância estatística de p&lt;0,05.</t>
+  </si>
+  <si>
+    <t>Posteriormente, cinco especialistas (um professor de saúde pública, um professor associado e um professor assistente de enfermagem em saúde pública, um professor associado de enfermagem em clínica médica e um professor assistente de saúde e enfermagem pediátrica) revisaram e forneceram opiniões sobre cada questão. O Índice de Validade de Conteúdo (IVC) foi usado para avaliar as opiniões dos especialistas. As frases em turco no instrumento foram pontuadas entre 1 e 4 com base em sua relevância e adequação para avaliar dor nas costas e postura: 1 = não apropriado, 2 = um pouco apropriado, 3 = apropriado e 4 = completamente apropriado (22,23). Os itens pontuados como 1 ou 2 foram revisados ​​e revisados. Por exemplo, a questão 6, que inicialmente pontuou 2 pontos, foi reformulada de "Você estuda/lê na cama?" para "Você estuda na cama?; Você lê livros na cama?". O IVC revisado resultou em uma pontuação alta de 90,8, indicando forte validade. A versão final em turco do instrumento foi retrotraduzida para o inglês por um professor de inglês, e não foram encontradas diferenças semânticas nas questões. Para testar a compreensibilidade, a ferramenta foi aplicada a 10 alunos semelhantes à população do estudo e foi considerada compreensível.</t>
+  </si>
+  <si>
+    <t>O método de análise fatorial exploratória é usado para testar a validade estrutural da ferramenta de avaliação e determinar os fatores. Se os dados obtidos do grupo de estudo são adequados para análise fatorial pode ser explicado com os testes Kaiser-Meyer-Olkin (KMO) e Barlett. Um valor de teste KMO menor que 0,50 é avaliado como uma análise fatorial não pode ser continuada (24). O teste de esfericidade de Barlett fornece o valor estatístico qui-quadrado; ele determina os fatores em um nível de significância menor que p &lt; 0,05. Se o valor de significância do teste de esfericidade de Barlett for maior que p&gt; 0,05, isso mostra que o nível de variância desejado não foi atingido e, portanto, a análise fatorial da escala não pode ser realizada (22). Neste estudo, a análise fatorial exploratória foi usada para a validade estrutural da ferramenta de avaliação e o valor de KMO foi encontrado em 0,374. Como esse valor é menor que 0,50, ele mostra que o conjunto de dados não é adequado para análise fatorial e a ferramenta de avaliação não pode ser dividida em fatores. Isso se deve ao fato de que a Ferramenta de Avaliação de Dor nas Costas e Postura não é uma escala do tipo Likert, mas sim um questionário que também inclui características sociodemográficas. A adequação do tamanho da amostra foi avaliada pelo Teste de Esfericidade de Bartlett (X = 464,7, p = 0,000). O valor de p significativo resultante do teste indica a adequação do tamanho da amostra.</t>
+  </si>
+  <si>
+    <t>O instrumento pode ser usado para avaliar a eficácia de intervenções voltadas para o tratamento da dor e da postura. Além disso, a ferramenta pode ser utilizada para identificar fatores potencialmente associados à dor em adolescentes.</t>
+  </si>
+  <si>
+    <t>Blocão da VAS
+Neste estudo, ela foi usada para avaliar a validade de critério da Ferramenta de Avaliação de Dor nas Costas e Postura, assumindo que haveria uma relação entre a pontuação de dor obtida pela EVA e os padrões de postura corporal.
+Na determinação da validade de critério, foi calculada a relação entre os escores obtidos na "VAS" medindo características semelhantes e a aplicação do mesmo grupo no mesmo momento, utilizando a análise de correlação de Pearson.
+Validade de critério: A validade de critério responde à questão de quão bem-sucedida a ferramenta de medição usada pode medir a característica que pretende medir (22). Neste estudo, a validade de critério foi avaliada com validade concorrente. A “Escala Visual Analógica (EVA)” foi usada para comparação. O coeficiente de correlação do teste de Spearman entre a questão “Presença de dor nas costas nos últimos 3 meses” na Ferramenta de Avaliação de Dor nas Costas e Postura Corporal e a pontuação da EVA foi determinado como r = -.684 (0,60-0,70), p = .000, e uma boa correlação negativa e relação significativa foi encontrada entre as duas ferramentas de medição. Este resultado mostra que as pontuações da EVA, que são aceitas como o teste padrão ouro, e as medições da Ferramenta de Avaliação de Dor nas Costas e Postura Corporal estão relacionadas e que esta ferramenta de avaliação pode medir a dor nas costas.</t>
   </si>
 </sst>
 </file>
@@ -1483,7 +1528,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1582,6 +1627,12 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1609,13 +1660,10 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1900,9 +1948,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F7" sqref="F7:F9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1944,13 +1992,13 @@
       </c>
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="38">
+      <c r="B2" s="40">
         <v>2013</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="37" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="3">
@@ -1970,9 +2018,9 @@
       </c>
     </row>
     <row r="3" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="38"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="35"/>
+      <c r="A3" s="40"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="37"/>
       <c r="D3" s="3">
         <v>2</v>
       </c>
@@ -1987,9 +2035,9 @@
       </c>
     </row>
     <row r="4" spans="1:8" s="3" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="A4" s="38"/>
-      <c r="B4" s="38"/>
-      <c r="C4" s="35"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="37"/>
       <c r="D4" s="3">
         <v>3</v>
       </c>
@@ -2004,9 +2052,9 @@
       </c>
     </row>
     <row r="5" spans="1:8" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="38"/>
-      <c r="B5" s="38"/>
-      <c r="C5" s="35"/>
+      <c r="A5" s="40"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="37"/>
       <c r="D5" s="3">
         <v>4</v>
       </c>
@@ -2017,9 +2065,9 @@
       <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="38"/>
-      <c r="B6" s="38"/>
-      <c r="C6" s="35"/>
+      <c r="A6" s="40"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="37"/>
       <c r="D6" s="3">
         <v>5</v>
       </c>
@@ -2030,16 +2078,16 @@
       <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:8" s="3" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="38"/>
-      <c r="B7" s="38"/>
-      <c r="C7" s="35"/>
+      <c r="A7" s="40"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="37"/>
       <c r="D7" s="3">
         <v>6</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="37" t="s">
+      <c r="F7" s="39" t="s">
         <v>25</v>
       </c>
       <c r="G7" s="4" t="s">
@@ -2047,37 +2095,37 @@
       </c>
     </row>
     <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="38"/>
-      <c r="B8" s="38"/>
-      <c r="C8" s="35"/>
+      <c r="A8" s="40"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="37"/>
       <c r="D8" s="3">
         <v>7</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="37"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:8" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="38"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="35"/>
+      <c r="A9" s="40"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="37"/>
       <c r="D9" s="3">
         <v>8</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="37"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="38"/>
-      <c r="B10" s="38"/>
-      <c r="C10" s="35"/>
+      <c r="A10" s="40"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="37"/>
       <c r="D10" s="3">
         <v>9</v>
       </c>
@@ -2090,9 +2138,9 @@
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="38"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="35"/>
+      <c r="A11" s="40"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="37"/>
       <c r="D11" s="3">
         <v>10</v>
       </c>
@@ -2103,9 +2151,9 @@
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:8" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="38"/>
-      <c r="B12" s="38"/>
-      <c r="C12" s="35"/>
+      <c r="A12" s="40"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="37"/>
       <c r="D12" s="3">
         <v>11</v>
       </c>
@@ -2120,9 +2168,9 @@
       </c>
     </row>
     <row r="13" spans="1:8" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A13" s="38"/>
-      <c r="B13" s="38"/>
-      <c r="C13" s="35"/>
+      <c r="A13" s="40"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="37"/>
       <c r="D13" s="3">
         <v>12</v>
       </c>
@@ -2158,13 +2206,13 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="36">
+      <c r="B15" s="38">
         <v>2018</v>
       </c>
-      <c r="C15" s="35" t="s">
+      <c r="C15" s="37" t="s">
         <v>40</v>
       </c>
       <c r="D15" s="3">
@@ -2173,7 +2221,7 @@
       <c r="E15" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="37" t="s">
+      <c r="F15" s="39" t="s">
         <v>46</v>
       </c>
       <c r="G15" s="4" t="s">
@@ -2184,39 +2232,39 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="36"/>
-      <c r="B16" s="36"/>
-      <c r="C16" s="35"/>
+      <c r="A16" s="38"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="37"/>
       <c r="D16" s="3">
         <v>2</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F16" s="37"/>
+      <c r="F16" s="39"/>
       <c r="G16" s="4" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="36"/>
-      <c r="B17" s="36"/>
-      <c r="C17" s="35"/>
+      <c r="A17" s="38"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="37"/>
       <c r="D17" s="3">
         <v>3</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F17" s="37"/>
+      <c r="F17" s="39"/>
       <c r="G17" s="4" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A18" s="36"/>
-      <c r="B18" s="36"/>
-      <c r="C18" s="35"/>
+      <c r="A18" s="38"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="37"/>
       <c r="D18" s="3">
         <v>4</v>
       </c>
@@ -2231,9 +2279,9 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="96" x14ac:dyDescent="0.25">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
-      <c r="C19" s="35"/>
+      <c r="A19" s="38"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="37"/>
       <c r="D19" s="3">
         <v>5</v>
       </c>
@@ -2248,9 +2296,9 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A20" s="36"/>
-      <c r="B20" s="36"/>
-      <c r="C20" s="35"/>
+      <c r="A20" s="38"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="37"/>
       <c r="D20" s="3">
         <v>6</v>
       </c>
@@ -2262,9 +2310,9 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A21" s="36"/>
-      <c r="B21" s="36"/>
-      <c r="C21" s="35"/>
+      <c r="A21" s="38"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="37"/>
       <c r="E21" s="4" t="s">
         <v>58</v>
       </c>
@@ -2299,13 +2347,13 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A23" s="36" t="s">
+      <c r="A23" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="B23" s="36">
+      <c r="B23" s="38">
         <v>2019</v>
       </c>
-      <c r="C23" s="35" t="s">
+      <c r="C23" s="37" t="s">
         <v>117</v>
       </c>
       <c r="E23" s="4" t="s">
@@ -2318,13 +2366,13 @@
         <v>120</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="36"/>
-      <c r="B24" s="36"/>
-      <c r="C24" s="35"/>
+      <c r="A24" s="38"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="37"/>
       <c r="E24" s="4" t="s">
         <v>63</v>
       </c>
@@ -2336,55 +2384,55 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="36"/>
-      <c r="B25" s="36"/>
-      <c r="C25" s="35"/>
+      <c r="A25" s="38"/>
+      <c r="B25" s="38"/>
+      <c r="C25" s="37"/>
       <c r="E25" s="4" t="s">
         <v>118</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="36"/>
-      <c r="B26" s="36"/>
-      <c r="C26" s="35"/>
+      <c r="A26" s="38"/>
+      <c r="B26" s="38"/>
+      <c r="C26" s="37"/>
       <c r="E26" s="4" t="s">
         <v>122</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>123</v>
+        <v>271</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="36"/>
-      <c r="B27" s="36"/>
-      <c r="C27" s="35"/>
+      <c r="A27" s="38"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="37"/>
       <c r="E27" s="4" t="s">
         <v>45</v>
       </c>
       <c r="F27" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="G27" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="G27" s="11" t="s">
-        <v>127</v>
-      </c>
     </row>
     <row r="28" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A28" s="34" t="s">
+      <c r="A28" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="B28" s="34">
+      <c r="B28" s="36">
         <v>2021</v>
       </c>
-      <c r="C28" s="35" t="s">
+      <c r="C28" s="37" t="s">
         <v>67</v>
       </c>
       <c r="E28" s="4" t="s">
@@ -2396,14 +2444,14 @@
       <c r="G28" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="H28" s="35" t="s">
+      <c r="H28" s="37" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A29" s="34"/>
-      <c r="B29" s="34"/>
-      <c r="C29" s="35"/>
+      <c r="A29" s="36"/>
+      <c r="B29" s="36"/>
+      <c r="C29" s="37"/>
       <c r="E29" s="4" t="s">
         <v>69</v>
       </c>
@@ -2413,12 +2461,12 @@
       <c r="G29" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="H29" s="35"/>
+      <c r="H29" s="37"/>
     </row>
     <row r="30" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="34"/>
-      <c r="B30" s="34"/>
-      <c r="C30" s="35"/>
+      <c r="A30" s="36"/>
+      <c r="B30" s="36"/>
+      <c r="C30" s="37"/>
       <c r="E30" s="4" t="s">
         <v>70</v>
       </c>
@@ -2428,7 +2476,7 @@
       <c r="G30" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="H30" s="35"/>
+      <c r="H30" s="37"/>
     </row>
     <row r="31" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -2633,11 +2681,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E623474-3705-4594-B9DF-AE0ADD157849}">
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B60" sqref="B60"/>
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A68" sqref="A68:A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2653,614 +2701,689 @@
     <row r="1" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16"/>
       <c r="B1" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="D1" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="E1" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="E1" s="20" t="s">
+    </row>
+    <row r="2" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A2" s="41" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="B2" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="D2" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="E2" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="C2" s="23" t="s">
+    </row>
+    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="41"/>
+      <c r="B3" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="C3" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D3" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4" s="41"/>
+      <c r="B4" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>177</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="41"/>
+      <c r="B5" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="41"/>
+      <c r="B6" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="41"/>
+      <c r="B7" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="41"/>
+      <c r="B8" s="22" t="s">
+        <v>188</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="41"/>
+      <c r="C9" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="41"/>
+      <c r="C10" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="41"/>
+      <c r="C11" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="41"/>
+      <c r="C12" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+      <c r="A13" s="41"/>
+      <c r="C13" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="E13" s="25" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="41"/>
+      <c r="C14" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="E14" s="25" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="41"/>
+      <c r="C15" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="E2" s="25" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="39"/>
-      <c r="B3" s="22" t="s">
-        <v>143</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="D3" s="24" t="s">
+      <c r="E15" s="25" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="41"/>
+      <c r="C16" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="E16" s="25" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="41"/>
+      <c r="C17" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="E17" s="25" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="41"/>
+      <c r="C18" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A19" s="41"/>
+      <c r="E19" s="25" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+      <c r="A20" s="41"/>
+      <c r="E20" s="25" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A21" s="41"/>
+      <c r="E21" s="25" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="41"/>
+      <c r="E22" s="25" t="s">
         <v>170</v>
       </c>
-      <c r="E3" s="25" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="39"/>
-      <c r="B4" s="22" t="s">
-        <v>144</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>136</v>
-      </c>
-      <c r="D4" s="24" t="s">
-        <v>178</v>
-      </c>
-      <c r="E4" s="25" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="39"/>
-      <c r="B5" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>139</v>
-      </c>
-      <c r="D5" s="24" t="s">
-        <v>179</v>
-      </c>
-      <c r="E5" s="25" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="39"/>
-      <c r="B6" s="22" t="s">
+    </row>
+    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="41"/>
+      <c r="E23" s="25" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="41"/>
+      <c r="E24" s="25" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="41"/>
+      <c r="E25" s="25" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="41"/>
+      <c r="E26" s="25" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A27" s="41"/>
+      <c r="E27" s="25" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A28" s="41"/>
+      <c r="E28" s="25" t="s">
         <v>181</v>
       </c>
-      <c r="C6" s="23" t="s">
-        <v>143</v>
-      </c>
-      <c r="E6" s="25" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="39"/>
-      <c r="B7" s="22" t="s">
-        <v>188</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>145</v>
-      </c>
-      <c r="E7" s="25" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="39"/>
-      <c r="B8" s="22" t="s">
-        <v>189</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>146</v>
-      </c>
-      <c r="E8" s="25" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="39"/>
-      <c r="C9" s="23" t="s">
-        <v>148</v>
-      </c>
-      <c r="E9" s="25" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="39"/>
-      <c r="C10" s="23" t="s">
-        <v>148</v>
-      </c>
-      <c r="E10" s="25" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="39"/>
-      <c r="C11" s="23" t="s">
-        <v>149</v>
-      </c>
-      <c r="E11" s="25" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="39"/>
-      <c r="C12" s="23" t="s">
-        <v>159</v>
-      </c>
-      <c r="E12" s="25" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="165" x14ac:dyDescent="0.25">
-      <c r="A13" s="39"/>
-      <c r="C13" s="23" t="s">
-        <v>160</v>
-      </c>
-      <c r="E13" s="25" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="39"/>
-      <c r="C14" s="23" t="s">
-        <v>161</v>
-      </c>
-      <c r="E14" s="25" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="39"/>
-      <c r="C15" s="23" t="s">
-        <v>164</v>
-      </c>
-      <c r="E15" s="25" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="39"/>
-      <c r="C16" s="23" t="s">
-        <v>175</v>
-      </c>
-      <c r="E16" s="25" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A17" s="39"/>
-      <c r="C17" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="E17" s="25" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="39"/>
-      <c r="C18" s="23" t="s">
-        <v>187</v>
-      </c>
-      <c r="E18" s="25" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A19" s="39"/>
-      <c r="E19" s="25" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="165" x14ac:dyDescent="0.25">
-      <c r="A20" s="39"/>
-      <c r="E20" s="25" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="135" x14ac:dyDescent="0.25">
-      <c r="A21" s="39"/>
-      <c r="E21" s="25" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="39"/>
-      <c r="E22" s="25" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="39"/>
-      <c r="E23" s="25" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="39"/>
-      <c r="E24" s="25" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="39"/>
-      <c r="E25" s="25" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="39"/>
-      <c r="E26" s="25" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="135" x14ac:dyDescent="0.25">
-      <c r="A27" s="39"/>
-      <c r="E27" s="25" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A28" s="39"/>
-      <c r="E28" s="25" t="s">
+    </row>
+    <row r="29" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A29" s="41"/>
+      <c r="E29" s="25" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A29" s="39"/>
-      <c r="E29" s="25" t="s">
+    <row r="30" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A30" s="41"/>
+      <c r="E30" s="25" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="135" x14ac:dyDescent="0.25">
-      <c r="A30" s="39"/>
-      <c r="E30" s="25" t="s">
+    <row r="31" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A31" s="41"/>
+      <c r="E31" s="25" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A31" s="39"/>
-      <c r="E31" s="25" t="s">
-        <v>185</v>
-      </c>
-    </row>
     <row r="32" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A32" s="40"/>
+      <c r="A32" s="42"/>
       <c r="B32" s="31"/>
       <c r="E32" s="27" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="150" x14ac:dyDescent="0.25">
-      <c r="A33" s="41" t="s">
+      <c r="A33" s="43" t="s">
+        <v>189</v>
+      </c>
+      <c r="B33" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="C33" s="29" t="s">
         <v>190</v>
       </c>
-      <c r="B33" s="30" t="s">
+      <c r="D33" s="28" t="s">
+        <v>200</v>
+      </c>
+      <c r="E33" s="26" t="s">
         <v>192</v>
       </c>
-      <c r="C33" s="29" t="s">
-        <v>191</v>
-      </c>
-      <c r="D33" s="28" t="s">
+    </row>
+    <row r="34" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A34" s="41"/>
+      <c r="B34" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="C34" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="D34" s="24" t="s">
         <v>201</v>
       </c>
-      <c r="E33" s="26" t="s">
+      <c r="E34" s="25" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A34" s="39"/>
-      <c r="B34" s="22" t="s">
-        <v>211</v>
-      </c>
-      <c r="C34" s="23" t="s">
+    <row r="35" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="41"/>
+      <c r="C35" s="23" t="s">
         <v>195</v>
       </c>
-      <c r="D34" s="24" t="s">
+      <c r="D35" s="24" t="s">
         <v>202</v>
       </c>
-      <c r="E34" s="25" t="s">
+      <c r="E35" s="25" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="39"/>
-      <c r="C35" s="23" t="s">
+    <row r="36" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="41"/>
+      <c r="C36" s="23" t="s">
         <v>196</v>
       </c>
-      <c r="D35" s="24" t="s">
+      <c r="E36" s="25" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A37" s="41"/>
+      <c r="C37" s="23" t="s">
+        <v>197</v>
+      </c>
+      <c r="E37" s="25" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="41"/>
+      <c r="C38" s="23" t="s">
         <v>203</v>
       </c>
-      <c r="E35" s="25" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="39"/>
-      <c r="C36" s="23" t="s">
-        <v>197</v>
-      </c>
-      <c r="E36" s="25" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A37" s="39"/>
-      <c r="C37" s="23" t="s">
-        <v>198</v>
-      </c>
-      <c r="E37" s="25" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="39"/>
-      <c r="C38" s="23" t="s">
+      <c r="E38" s="25" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+      <c r="A39" s="41"/>
+      <c r="C39" s="23" t="s">
         <v>204</v>
       </c>
-      <c r="E38" s="25" t="s">
+      <c r="E39" s="25" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="180" x14ac:dyDescent="0.25">
-      <c r="A39" s="39"/>
-      <c r="C39" s="23" t="s">
-        <v>205</v>
-      </c>
-      <c r="E39" s="25" t="s">
+    <row r="40" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A40" s="41"/>
+      <c r="E40" s="25" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A40" s="39"/>
-      <c r="E40" s="25" t="s">
+    <row r="41" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="41"/>
+      <c r="E41" s="25" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" s="39"/>
-      <c r="E41" s="25" t="s">
-        <v>209</v>
-      </c>
-    </row>
     <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="40"/>
+      <c r="A42" s="42"/>
       <c r="D42" s="33"/>
       <c r="E42" s="27" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="300" x14ac:dyDescent="0.25">
-      <c r="A43" s="41" t="s">
-        <v>212</v>
+      <c r="A43" s="43" t="s">
+        <v>211</v>
       </c>
       <c r="B43" s="32"/>
       <c r="C43" s="29" t="s">
+        <v>213</v>
+      </c>
+      <c r="D43" s="24" t="s">
+        <v>215</v>
+      </c>
+      <c r="E43" s="25" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+      <c r="A44" s="44"/>
+      <c r="C44" s="23" t="s">
         <v>214</v>
       </c>
-      <c r="D43" s="24" t="s">
+      <c r="D44" s="24" t="s">
         <v>216</v>
       </c>
-      <c r="E43" s="25" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="180" x14ac:dyDescent="0.25">
-      <c r="A44" s="42"/>
-      <c r="C44" s="23" t="s">
-        <v>215</v>
-      </c>
-      <c r="D44" s="24" t="s">
+    </row>
+    <row r="45" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45" s="44"/>
+      <c r="B45" s="31"/>
+      <c r="C45" s="34" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="42"/>
-      <c r="B45" s="31"/>
-      <c r="C45" s="43" t="s">
+    <row r="46" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A46" s="43" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A46" s="44" t="s">
+      <c r="B46" s="22" t="s">
         <v>219</v>
       </c>
-      <c r="B46" s="22" t="s">
+      <c r="C46" s="23" t="s">
         <v>220</v>
       </c>
-      <c r="C46" s="23" t="s">
+      <c r="D46" s="28" t="s">
+        <v>239</v>
+      </c>
+      <c r="E46" s="35" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+      <c r="A47" s="41"/>
+      <c r="B47" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="D46" s="28" t="s">
+      <c r="C47" s="23" t="s">
+        <v>223</v>
+      </c>
+      <c r="D47" s="24" t="s">
         <v>240</v>
       </c>
-      <c r="E46" s="45" t="s">
+      <c r="E47" s="25" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="165" x14ac:dyDescent="0.25">
-      <c r="B47" s="22" t="s">
+    <row r="48" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A48" s="41"/>
+      <c r="B48" s="22" t="s">
         <v>222</v>
       </c>
-      <c r="C47" s="23" t="s">
+      <c r="C48" s="23" t="s">
+        <v>227</v>
+      </c>
+      <c r="E48" s="25" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A49" s="41"/>
+      <c r="B49" s="22" t="s">
         <v>224</v>
       </c>
-      <c r="D47" s="24" t="s">
+      <c r="C49" s="23" t="s">
+        <v>236</v>
+      </c>
+      <c r="E49" s="25" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A50" s="41"/>
+      <c r="B50" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="C50" s="23" t="s">
+        <v>237</v>
+      </c>
+      <c r="E50" s="25" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A51" s="41"/>
+      <c r="B51" s="22" t="s">
+        <v>250</v>
+      </c>
+      <c r="C51" s="23" t="s">
+        <v>251</v>
+      </c>
+      <c r="E51" s="25" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A52" s="41"/>
+      <c r="B52" s="22" t="s">
+        <v>252</v>
+      </c>
+      <c r="C52" s="23" t="s">
+        <v>255</v>
+      </c>
+      <c r="E52" s="25" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A53" s="41"/>
+      <c r="B53" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="C53" s="23" t="s">
+        <v>257</v>
+      </c>
+      <c r="E53" s="25" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A54" s="41"/>
+      <c r="B54" s="22" t="s">
+        <v>258</v>
+      </c>
+      <c r="C54" s="23" t="s">
+        <v>264</v>
+      </c>
+      <c r="E54" s="25" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A55" s="41"/>
+      <c r="B55" s="22" t="s">
+        <v>259</v>
+      </c>
+      <c r="E55" s="25" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A56" s="41"/>
+      <c r="B56" s="22" t="s">
+        <v>261</v>
+      </c>
+      <c r="E56" s="25" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A57" s="41"/>
+      <c r="B57" s="22" t="s">
+        <v>262</v>
+      </c>
+      <c r="E57" s="25" t="s">
         <v>241</v>
       </c>
-      <c r="E47" s="25" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="135" x14ac:dyDescent="0.25">
-      <c r="B48" s="22" t="s">
-        <v>223</v>
-      </c>
-      <c r="C48" s="23" t="s">
-        <v>228</v>
-      </c>
-      <c r="E48" s="25" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="B49" s="22" t="s">
-        <v>225</v>
-      </c>
-      <c r="C49" s="23" t="s">
-        <v>237</v>
-      </c>
-      <c r="E49" s="25" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B50" s="22" t="s">
+    </row>
+    <row r="58" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+      <c r="A58" s="41"/>
+      <c r="B58" s="22" t="s">
+        <v>263</v>
+      </c>
+      <c r="E58" s="25" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A59" s="41"/>
+      <c r="B59" s="22" t="s">
+        <v>265</v>
+      </c>
+      <c r="E59" s="25" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="41"/>
+      <c r="E60" s="25" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A61" s="41"/>
+      <c r="E61" s="25" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A62" s="41"/>
+      <c r="E62" s="25" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="41"/>
+      <c r="E63" s="25" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A64" s="41"/>
+      <c r="E64" s="25" t="s">
         <v>249</v>
       </c>
-      <c r="C50" s="23" t="s">
-        <v>238</v>
-      </c>
-      <c r="E50" s="25" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B51" s="22" t="s">
-        <v>251</v>
-      </c>
-      <c r="C51" s="23" t="s">
-        <v>252</v>
-      </c>
-      <c r="E51" s="25" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="B52" s="22" t="s">
-        <v>253</v>
-      </c>
-      <c r="C52" s="23" t="s">
+    </row>
+    <row r="65" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A65" s="41"/>
+      <c r="E65" s="25" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A66" s="41"/>
+      <c r="E66" s="25" t="s">
         <v>256</v>
       </c>
-      <c r="E52" s="25" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="53" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B53" s="22" t="s">
-        <v>254</v>
-      </c>
-      <c r="C53" s="23" t="s">
-        <v>258</v>
-      </c>
-      <c r="E53" s="25" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="54" spans="2:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="B54" s="22" t="s">
-        <v>259</v>
-      </c>
-      <c r="C54" s="23" t="s">
-        <v>265</v>
-      </c>
-      <c r="E54" s="25" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="55" spans="2:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="B55" s="22" t="s">
+    </row>
+    <row r="67" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A67" s="41"/>
+      <c r="B67" s="31"/>
+      <c r="E67" s="25" t="s">
         <v>260</v>
       </c>
-      <c r="E55" s="25" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="56" spans="2:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="B56" s="22" t="s">
-        <v>262</v>
-      </c>
-      <c r="E56" s="25" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="57" spans="2:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B57" s="22" t="s">
-        <v>263</v>
-      </c>
-      <c r="E57" s="25" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="58" spans="2:5" ht="165" x14ac:dyDescent="0.25">
-      <c r="B58" s="22" t="s">
-        <v>264</v>
-      </c>
-      <c r="E58" s="25" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="59" spans="2:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B59" s="22" t="s">
+    </row>
+    <row r="68" spans="1:5" ht="210" x14ac:dyDescent="0.25">
+      <c r="A68" s="45" t="s">
+        <v>267</v>
+      </c>
+      <c r="B68" s="22" t="s">
+        <v>268</v>
+      </c>
+      <c r="C68" s="29" t="s">
         <v>266</v>
       </c>
-      <c r="E59" s="25" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="60" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="E60" s="25" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="61" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="E61" s="25" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="62" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="E62" s="25" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="63" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="E63" s="25" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="64" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="E64" s="25" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="65" spans="5:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="E65" s="25" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="66" spans="5:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="E66" s="25" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="67" spans="5:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="E67" s="25" t="s">
-        <v>261</v>
+      <c r="D68" s="28" t="s">
+        <v>268</v>
+      </c>
+      <c r="E68" s="35" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="255" x14ac:dyDescent="0.25">
+      <c r="A69" s="46"/>
+      <c r="B69" s="22" t="s">
+        <v>269</v>
+      </c>
+      <c r="C69" s="23" t="s">
+        <v>270</v>
+      </c>
+      <c r="E69" s="25" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="315" x14ac:dyDescent="0.25">
+      <c r="A70" s="46"/>
+      <c r="B70" s="22" t="s">
+        <v>277</v>
+      </c>
+      <c r="C70" s="23" t="s">
+        <v>273</v>
+      </c>
+      <c r="E70" s="25" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="360" x14ac:dyDescent="0.25">
+      <c r="A71" s="46"/>
+      <c r="C71" s="23" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="C72" s="23" t="s">
+        <v>278</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A2:A32"/>
     <mergeCell ref="A33:A42"/>
     <mergeCell ref="A43:A45"/>
+    <mergeCell ref="A46:A67"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Tabela descritiva das fontes
Revisão e alteração da tabela descritiva das fontes
</commit_message>
<xml_diff>
--- a/Extração dos dados.xlsx
+++ b/Extração dos dados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pichau\Documents\ProjetosTese\10-anos-de-back-pei\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909AD316-09B6-4A89-A1A9-DEA90D68C6CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A965C7A-845F-4152-9A9B-07670A798769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="16305" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Descritivos" sheetId="1" r:id="rId1"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="581">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="642">
   <si>
     <t>Autor</t>
   </si>
@@ -2089,12 +2089,6 @@
     <t xml:space="preserve">O sistema de medição que pretende mensurar o comportamento de cuidado com as costas entre crianças do ensino fundamental deveria abordar os constructos propostos pela Teoria Cognitiva Social que aponta que os três principais determinantes psicológicos de qualquer mudança de comportamento são: autoeficácia; capacidade comportamental (habilidades e conhecimento para executar um determinado comportamento); e crenças de expectativa de resultados (crenças comportamentais). O sistema de medição é composto por 5 construtos: habilidades, autoeficácia, conhecimento, crenças de expectativa e comportamento auto-relatado. Um painel de especialista avaliou os itens quanto a sua necessidade e relevância. A associação dos itens com os construtos foi verificada por um correlação item-total. Foi executada uma análise fatorial e para investigar os construtos e um procedimento de validade convergente pra verificar as relações entre eles. O alfa de Cronbach foi usado para verificar a consistência interna.  </t>
   </si>
   <si>
-    <t>≥</t>
-  </si>
-  <si>
-    <t>≤</t>
-  </si>
-  <si>
     <t>Cada construto possui uma representação própria. Habilidades: cada item é classificado em uma escala de 3 pontos que varia de 0 (não cumprimento dos critérios) a 2 (conclusão correta da tarefa), dando uma pontuação que varia de 0 a 48 pontos, onde pontuações mais altas indicam melhor cumprimento das tarefas. Conhecimento: as pontuações neste constructo variam de 0 a 13, onde as pontuações mais altas indicam melhor conhecimento. Autoeficácia: cada item é classificado em uma escala de quatro pontos (de difícil a fácil), dando uma pontuação que varia de 4 a 16, onde as pontuações mais altas indicam maior autoeficácia. Crenças de expectativa: cada item é classificado em uma escala de cinco pontos (discordo totalmente a concordo totalmente), dando uma pontuação que varia de 6 a 30, onde uma pontuação mais alta indica crenças mais fortes. Comportamento de cuidado com as costas: as categorias de resposta variaram de nunca (1) a sempre (5), dando uma pontuação de 8 a 40, onde pontuações mais altas indicam melhor comportamento preventivo. Os valores dos construtos podem ser somados gerando uma representação para o sistema de medição que varia de 16 a 132. Os critérios para interpretar as pontuações são: alta (≥104); intermediária (entre o primeiro e o terceiro quartel, ≥45 e ≤103); e baixa (≤44). Foi calculado o MDC.</t>
   </si>
   <si>
@@ -2245,9 +2239,6 @@
     <t>Elaboração dos itens relativos aos fatores de risco.</t>
   </si>
   <si>
-    <t>Painel com 8 especialistas avaliaram: adequação ao avaliar AVDs a partir de fotografias; adequação ao avaliar dor nas costas e fatores associados; a clareza, facilidade de compreensão e aplicabilidade. Avaliação através de tabelas de frequência.</t>
-  </si>
-  <si>
     <t>Recomendações: melhor estruturação das questões; melhorar a qualidade das imagens; alterar algumas imagens; preparar uma versão para cada gênero com posturas diferentes. Aprovação do sistema de medição na segunda rodada de consulta ao painel.</t>
   </si>
   <si>
@@ -2260,20 +2251,10 @@
     <t>Não havia necesidade de mudanças</t>
   </si>
   <si>
-    <t>Validade de conteúdo e elaboração do questionário</t>
-  </si>
-  <si>
     <t>Versão em inglês do questionário</t>
   </si>
   <si>
-    <t>Tradução independente por 3 tradutores. Análise da equivalência semântica, cultural e conceitual por um painel de especialistas.</t>
-  </si>
-  <si>
     <t>Confiabilidade teste-reteste (reprodutibilidade através de um procedimento de teste e reteste)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verificar se existe consistência entre os resultados de dois instrumentos para avaliar a postura corporal durante AVDs, o BackPEI e o LADy, em estudantes de 11 a 15 anos
-</t>
   </si>
   <si>
     <r>
@@ -2346,32 +2327,325 @@
     <t>Revisão de literatura e experiência das autoras para identificar fatores de risco para dor nas costas e pescoço entre adultos</t>
   </si>
   <si>
-    <t xml:space="preserve">Painel com 3 especialistas avaliaram: adequação ao avaliar AVDs a partir de fotografias; adequação ao avaliar dor nas costas e no pescoço e fatores associados; a clareza, facilidade de compreensão e aplicabilidade. </t>
-  </si>
-  <si>
     <t>Especialistas recomendaram pequenas alterações que foram realizadas. Na segunda rodada de consulta constatou-se que não seria preciso nenhuma alteração</t>
   </si>
   <si>
     <t>Confiabilidade teste-reteste (Reprodutibilidade)</t>
   </si>
   <si>
-    <t>O questionário foi aplicado duas vezes em 260 indivíduos com intervalo de 7 dias. A avaliação ocorreu através do κnão ponderado (≥0,5), CCI e teste dos postos de sinais de Wilcoxon (p&gt;0,05).</t>
-  </si>
-  <si>
     <t>Todos os itens apresentaram κ&gt;0,5. A intensidade da dor obteve CCI=0,937 com diferença não-significativa segundo o teste dos postos de sinais de Wilcoxon (p=0,251). .</t>
   </si>
   <si>
-    <t>O questionário foi aplicado duas vezes em 154 indivíduos com intervalo de 7 dias. A avaliação ocorreu através do κ (≥0,5), CCI2,2.</t>
-  </si>
-  <si>
-    <t>Todos os itens apresentaram κ&gt;0,5. A intensidade da dor apresentou CCI=0,908, para dor nas costas, e CCI=0,865, para dor no pescoço.</t>
+    <t>Envolve apenas as questões referentes aos fatores de risco. Obtida pela soma dos pontos (máximo de 10 pontos). Quanto maior o valor, menor a exposição a fatores de risco.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Envolve apenas as questões referentes aos fatores de risco. Obtida pela soma dos pontos (máximo de 16 pontos). Quanto maior o valor, menor a exposição a fatores de risco. </t>
+  </si>
+  <si>
+    <t>Tradução independente por 3 tradutores. Análise da equivalência semântica, cultural e conceitual por um painel de 2 especialistas.</t>
+  </si>
+  <si>
+    <t>Validade de Conteúdo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tradução para o turco </t>
+  </si>
+  <si>
+    <t>Validade de linguagem</t>
+  </si>
+  <si>
+    <t>O questinário foi retraduzido para o inglês para verificar se houve alteração do significado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 tradutor realizou a tradução do inglês para o turco, outro tradutor avaliou a compreensão e gramática. </t>
+  </si>
+  <si>
+    <t>Painel com 5 especialistas verificaram a clareza, relevância e adequação de cada questão. Avaliação através do IVC.</t>
+  </si>
+  <si>
+    <t>Versão preliminar do questionário em turco</t>
+  </si>
+  <si>
+    <t>Não houve alteração do significado das questões</t>
+  </si>
+  <si>
+    <t>O questionário foi aplicado entre 139 estudantes e foi avaliado através dos valores de KMO e do teste de esfericidade de Bartlett.</t>
+  </si>
+  <si>
+    <t>Validade convergente (validade de critério)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O questionário foi aplicado entre 139 estudantes. Voi analisada a associação entre a intensidade da dor nas costas e a presença de dor nas costas através do </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>ρ</t>
+    </r>
+  </si>
+  <si>
+    <t>ρ=-0,684</t>
+  </si>
+  <si>
+    <t>Avaliação da compreensão do questionário</t>
+  </si>
+  <si>
+    <t>O questionário foi aplicado entre 10 estudantes de perfil similar à população do estudo</t>
+  </si>
+  <si>
+    <t>O questionário foi aplicado duas vezes entre 154 indivíduos com intervalo de 7 dias. A avaliação ocorreu através do κ (≥0,5), CCI2,2.</t>
+  </si>
+  <si>
+    <t>O questionário foi aplicado duas vezes entre 260 indivíduos com intervalo de 7 dias. A avaliação ocorreu através do κnão ponderado (≥0,5), CCI e teste dos postos de sinais de Wilcoxon (p&gt;0,05).</t>
+  </si>
+  <si>
+    <t>A avaliação ocorreu através do κ e testes dos postos de sinal de Wilcoxon.</t>
+  </si>
+  <si>
+    <t>Um tradutor traduziu do português para o espanhol. Um segundo tradutorretraduziu do espanhol para o português. Um terceiro tradutor comparou a versão traduzida para o espanhol e retraduzida para o português. A versão preliminar foi estabelecida por consenso entre os três tradutores.</t>
+  </si>
+  <si>
+    <t>Nenhuma intervenção foi feita. Questionário retraduzido  para o português era idêntico ao original em português.</t>
+  </si>
+  <si>
+    <t>Painel com 2 especialistas verificaram a equivalência da versão em espanhol quanto asemântica, idiomática, experiencial e conceitual. Erros de revisão foram corrigidos. Avaliação ocorreu através da concordância (≥80%).</t>
+  </si>
+  <si>
+    <t>A 2ª rodada já resultou em consenso, entretanto, acolheu-se novas sugestões feitas. Na 3ª rodada houve 100% de concordância em todos os itens. Não foram encontrados erros na revisão.</t>
+  </si>
+  <si>
+    <t>O questionário foi aplicado duas vezes entre 224 indivíduos com intervalo de 7 dias. A avaliação ocorreu através do ICC (≥0,75), teste dos postos de sinais de Wilcoxon e κ com %C (κ≥0,5 ou %C≥75%).</t>
+  </si>
+  <si>
+    <t>2 itens com κ&lt;0,5 e 4 itens com %C&lt;75%, nenhum inferior em ambos. A inteisidade da dor obteve ICC=0,928, sem diferença significativa segundo Wilcoxon.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revisão de literatura para identificar como a dor nas costas é avaliada e fatores de risco </t>
+  </si>
+  <si>
+    <t>Versão preliminar do questionário do BackPEI-CA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Painel com 3 especialistas avaliou: adequação ao avaliar AVDs a partir de fotografias; adequação ao avaliar dor nas costas e no pescoço e fatores associados; a clareza, facilidade de compreensão e aplicabilidade. </t>
+  </si>
+  <si>
+    <t>Painel com 8 especialistas avaliou: adequação ao avaliar AVDs a partir de fotografias; adequação ao avaliar dor nas costas e fatores associados; a clareza, facilidade de compreensão e aplicabilidade. Avaliação através de tabelas de frequência.</t>
+  </si>
+  <si>
+    <t>O questionário foi aplicado duas vezes entre 105 indivíduos com intervalo de 7 dias no formato presencial e virtual. A avaliação ocorreu através do %C (&gt;50%), κ (≥0,4) e CCI(2-way mixed effects absolute agrement)</t>
+  </si>
+  <si>
+    <t>Todos os itens apresentaram %C&gt;50% e κ&gt;0,4. A intensidade da dor apresentou CCI=0,828 para dor nas costas e CCI=0,824 para dor no pescoço.</t>
+  </si>
+  <si>
+    <t>Todos os itens apresentaram κ&gt;0,5. A intensidade da dor apresentou CCI=0,908 para dor nas costas e CCI=0,865, para dor no pescoço.</t>
+  </si>
+  <si>
+    <t>Versão em inglês do questionário do BackPEI-CA</t>
+  </si>
+  <si>
+    <t>Inclusão de questões novas</t>
+  </si>
+  <si>
+    <t>Painel com 8 especialistas analisaram: clareza, facilidade de compreensão e aplicabilidade geral das novas questões; se as novas questões permitiam a identificação do comportamento de uso de dispositivos móveis; se a nova versão avaliava adequadamente dor nas costas e no pescoço. A avaliação aconteceu através do IVC para cada questão (&gt;0,8, preferencialmente &gt;0,9).</t>
+  </si>
+  <si>
+    <t>Painel com 8 especialistas avaliou:  clareza, facilidade de compreensão e aplicabilidade das novas questões e novo design; se as novas questões permitem a identificação dos fatores comportamentais relativos ao uso de dispositivos móveis. A avaliação aconteceu através do IVC para cada questão (≥0,8).</t>
+  </si>
+  <si>
+    <t>Na 2ª rodada foram obtidos ICV=1 para novas questões e design e ICV = 0,87 para os fatores comportamentais. Elaboração da versão final do BackPEI-A</t>
+  </si>
+  <si>
+    <t>O item referenet a ler e/ou estudar na cama foi separada em 2: ler na cama; e estudar na cama. Obteve-se um IVC=0,908. Elaboração da versão final do questionário em turco do BackPEI.</t>
+  </si>
+  <si>
+    <t>Na 2ª rododa o ICV variou de 0,9 a 1,0. Elaboração da versao final do BackPEI-CA</t>
+  </si>
+  <si>
+    <t>O questionário foi aplicado duas vezes entre 194 indivíduos com intervalo de 7 dias no formato presencial (n=89) e virtual (n=105). A avaliação ocorreu através do %C (&gt;50%), κ (&gt;0,4) e CCI2,2, EPM, MMD</t>
+  </si>
+  <si>
+    <t>Todos os itens apresentaram %C&gt;50% e κ&gt;0,4. A intensidade da dor nas costas apresentou CCI=0,595, SEM=1,26cm e MMD=2,48cm. A intensidade de dor no pescoço apresentou CCI=0,479, SEM=1,68cm e MMD=3,10cm.</t>
+  </si>
+  <si>
+    <t>Versão em inglês do questionário do BackPEI-A</t>
+  </si>
+  <si>
+    <t>Confiabilidade teste-reteste (Consistência interna - a parte do kappa e %C)</t>
+  </si>
+  <si>
+    <t>Todos os itens apresentaram κ&gt;0,5, %C e EP variaram respectivamente de 74,5% a 100% e 0,000 a 0,138. A intensidade da dor nas costas apresentou CCI=0,716. A intensidade de dor no pescoço apresentou CCI=0,944. A pontuação total do BackPEI apresentou CCI=0,800, r=0,809 e diferença significativa segundo o teste dos postos de sinais de Wilcoxon (p=0,009).</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>O questionário foi aplicado duas vezes entre 235 indivíduos com intervalo de 7 dias. A avaliação ocorreu através do κ (≥0,5), %C, EP, CCI (2-way random effects - absolute agreement), r, teste dos postos de sinais de Wilcoxon.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>0,5), %C e SE</t>
+    </r>
+  </si>
+  <si>
+    <t>Validade convergente (validade concorrente)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O BackPEI-TR e o MHQ-TR foram aplicados entre 235 indivíduos. A avaliação ocorreu a partir do ρ. </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>ρ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>=0,725.</t>
+    </r>
+  </si>
+  <si>
+    <t>A partir da pontuação do BackPEI obtida entre 235 indivíduos foram determinados dois grupos: aqueles com valores acima do 73º percentil (G&gt;73º); e aqueles com valores abaixo do 23º percentil (G&lt;23º). Os valores dos grupos foram comparados através do teste t independente.</t>
+  </si>
+  <si>
+    <t>Diferença significativa segundo o teste t (p&lt;0,001)</t>
+  </si>
+  <si>
+    <t>Painel com 13 especialistas avaliou a utilidade e relevância de cada item. A avaliação aconteceu através do IVC (&gt;0,7) e RVC (≥0,54).</t>
+  </si>
+  <si>
+    <t>4 itens foram excluídos. Elaboração da versão intermediária do BABAQ.</t>
+  </si>
+  <si>
+    <t>Avaliação qualitativa da compreensão do questionário (Validade de face)</t>
+  </si>
+  <si>
+    <t>2 itens foram excluídos. Elaboração da versão final do BABAQ.</t>
+  </si>
+  <si>
+    <t>O questionário foi aplicado entre 6 alunas da 5ª série que avaliaram se conseguiam ler e entender as questões.</t>
+  </si>
+  <si>
+    <t>O questionário do BABAQ foi aplicado entre 610 indivíduos. Foi realizada uma Análise Fatorial Confimartória. A avaliação ocorreu através da χ²/gl (&lt;5), CFI, RMSEA (&lt;0,10), SRMR (&lt;0,08) e correlação item-total</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>χ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>²/gl</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=3,51; ICA=0,97; RMSEA=0,091; SRMR=0,078; correlação item-total  satisfatória;</t>
+    </r>
+  </si>
+  <si>
+    <t>Variância Média Extraída (&gt;0,5)</t>
+  </si>
+  <si>
+    <t>O questionário foi aplicado duas vezes entre 50 indivíduos com intervalo de 2 semanas. A avaliação ocorreu através do α (&gt;0,70), ICC (&gt;0,70), EPM e MMD</t>
+  </si>
+  <si>
+    <t>α entre 0,93 e 0,97, ICC entre 0,76 e 0,83,  EPM entre 0,72 e 7,08 e MMD entre 1,99 e 19,62</t>
+  </si>
+  <si>
+    <t>Noll et al. (2013)</t>
+  </si>
+  <si>
+    <t>Antoniolli et al. (2015)</t>
+  </si>
+  <si>
+    <t>Pivotto et al. (2018)</t>
+  </si>
+  <si>
+    <t>Candotti et al. (2018)</t>
+  </si>
+  <si>
+    <t>Gençbas e Bebis (2019)</t>
+  </si>
+  <si>
+    <t>Akbari-Chehrehbargh, Tavafian e Montazeri (2020)</t>
+  </si>
+  <si>
+    <t>Miñana-Signes et al. (2021)</t>
+  </si>
+  <si>
+    <t>Rosa et al. (2022)</t>
+  </si>
+  <si>
+    <t>Candotti et al. (2023)</t>
+  </si>
+  <si>
+    <r>
+      <t>Gök</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>ş</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>en, Kocaman e Yildirim (2023)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2455,8 +2729,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2493,12 +2779,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -2530,7 +2810,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2641,7 +2921,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -2658,40 +2937,31 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -2705,15 +2975,23 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2997,25 +3275,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:H52"/>
+    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="41" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" style="40" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="76" style="2" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="3"/>
     <col min="5" max="5" width="50.5703125" style="4" customWidth="1"/>
     <col min="6" max="6" width="70.7109375" style="5" customWidth="1"/>
     <col min="7" max="7" width="55.42578125" style="4" customWidth="1"/>
     <col min="8" max="8" width="39.7109375" style="3" customWidth="1"/>
-    <col min="9" max="12" width="36.5703125" style="43" customWidth="1"/>
+    <col min="9" max="12" width="36.5703125" style="42" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -3039,27 +3317,27 @@
       <c r="H1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="42" t="s">
+      <c r="I1" s="41" t="s">
         <v>128</v>
       </c>
-      <c r="J1" s="42" t="s">
+      <c r="J1" s="41" t="s">
         <v>129</v>
       </c>
-      <c r="K1" s="42" t="s">
+      <c r="K1" s="41" t="s">
         <v>130</v>
       </c>
-      <c r="L1" s="42" t="s">
+      <c r="L1" s="41" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="3" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="53">
+      <c r="B2" s="49">
         <v>2013</v>
       </c>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="46" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="3">
@@ -3077,23 +3355,23 @@
       <c r="H2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="48" t="s">
+      <c r="I2" s="50" t="s">
         <v>450</v>
       </c>
-      <c r="J2" s="48" t="s">
+      <c r="J2" s="50" t="s">
         <v>489</v>
       </c>
-      <c r="K2" s="48" t="s">
+      <c r="K2" s="50" t="s">
         <v>451</v>
       </c>
-      <c r="L2" s="48" t="s">
+      <c r="L2" s="50" t="s">
         <v>490</v>
       </c>
     </row>
     <row r="3" spans="1:12" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="50"/>
-      <c r="B3" s="53"/>
-      <c r="C3" s="52"/>
+      <c r="A3" s="44"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="46"/>
       <c r="D3" s="3">
         <v>2</v>
       </c>
@@ -3106,15 +3384,15 @@
       <c r="G3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="48"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="48"/>
-      <c r="L3" s="48"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="50"/>
     </row>
     <row r="4" spans="1:12" s="3" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="A4" s="50"/>
-      <c r="B4" s="53"/>
-      <c r="C4" s="52"/>
+      <c r="A4" s="44"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="46"/>
       <c r="D4" s="3">
         <v>3</v>
       </c>
@@ -3127,15 +3405,15 @@
       <c r="G4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="48"/>
-      <c r="J4" s="48"/>
-      <c r="K4" s="48"/>
-      <c r="L4" s="48"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="50"/>
     </row>
     <row r="5" spans="1:12" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="50"/>
-      <c r="B5" s="53"/>
-      <c r="C5" s="52"/>
+      <c r="A5" s="44"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="46"/>
       <c r="D5" s="3">
         <v>4</v>
       </c>
@@ -3144,15 +3422,15 @@
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="4"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="48"/>
-      <c r="K5" s="48"/>
-      <c r="L5" s="48"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="50"/>
+      <c r="K5" s="50"/>
+      <c r="L5" s="50"/>
     </row>
     <row r="6" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="50"/>
-      <c r="B6" s="53"/>
-      <c r="C6" s="52"/>
+      <c r="A6" s="44"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="46"/>
       <c r="D6" s="3">
         <v>5</v>
       </c>
@@ -3161,72 +3439,72 @@
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="4"/>
-      <c r="I6" s="48"/>
-      <c r="J6" s="48"/>
-      <c r="K6" s="48"/>
-      <c r="L6" s="48"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="50"/>
+      <c r="K6" s="50"/>
+      <c r="L6" s="50"/>
     </row>
     <row r="7" spans="1:12" s="3" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="50"/>
-      <c r="B7" s="53"/>
-      <c r="C7" s="52"/>
+      <c r="A7" s="44"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="46"/>
       <c r="D7" s="3">
         <v>6</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="51" t="s">
+      <c r="F7" s="48" t="s">
         <v>25</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="I7" s="48"/>
-      <c r="J7" s="48"/>
-      <c r="K7" s="48"/>
-      <c r="L7" s="48"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
     </row>
     <row r="8" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="50"/>
-      <c r="B8" s="53"/>
-      <c r="C8" s="52"/>
+      <c r="A8" s="44"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="46"/>
       <c r="D8" s="3">
         <v>7</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="51"/>
+      <c r="F8" s="48"/>
       <c r="G8" s="4"/>
-      <c r="I8" s="48"/>
-      <c r="J8" s="48"/>
-      <c r="K8" s="48"/>
-      <c r="L8" s="48"/>
+      <c r="I8" s="50"/>
+      <c r="J8" s="50"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="50"/>
     </row>
     <row r="9" spans="1:12" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="50"/>
-      <c r="B9" s="53"/>
-      <c r="C9" s="52"/>
+      <c r="A9" s="44"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="46"/>
       <c r="D9" s="3">
         <v>8</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="51"/>
+      <c r="F9" s="48"/>
       <c r="G9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="I9" s="48"/>
-      <c r="J9" s="48"/>
-      <c r="K9" s="48"/>
-      <c r="L9" s="48"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="50"/>
+      <c r="K9" s="50"/>
+      <c r="L9" s="50"/>
     </row>
     <row r="10" spans="1:12" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="50"/>
-      <c r="B10" s="53"/>
-      <c r="C10" s="52"/>
+      <c r="A10" s="44"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="46"/>
       <c r="D10" s="3">
         <v>9</v>
       </c>
@@ -3237,15 +3515,15 @@
         <v>24</v>
       </c>
       <c r="G10" s="4"/>
-      <c r="I10" s="48"/>
-      <c r="J10" s="48"/>
-      <c r="K10" s="48"/>
-      <c r="L10" s="48"/>
+      <c r="I10" s="50"/>
+      <c r="J10" s="50"/>
+      <c r="K10" s="50"/>
+      <c r="L10" s="50"/>
     </row>
     <row r="11" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="50"/>
-      <c r="B11" s="53"/>
-      <c r="C11" s="52"/>
+      <c r="A11" s="44"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="46"/>
       <c r="D11" s="3">
         <v>10</v>
       </c>
@@ -3254,15 +3532,15 @@
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="4"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="48"/>
-      <c r="K11" s="48"/>
-      <c r="L11" s="48"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="50"/>
+      <c r="L11" s="50"/>
     </row>
     <row r="12" spans="1:12" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="50"/>
-      <c r="B12" s="53"/>
-      <c r="C12" s="52"/>
+      <c r="A12" s="44"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="46"/>
       <c r="D12" s="3">
         <v>11</v>
       </c>
@@ -3275,15 +3553,15 @@
       <c r="G12" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="I12" s="48"/>
-      <c r="J12" s="48"/>
-      <c r="K12" s="48"/>
-      <c r="L12" s="48"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="50"/>
     </row>
     <row r="13" spans="1:12" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A13" s="50"/>
-      <c r="B13" s="53"/>
-      <c r="C13" s="52"/>
+      <c r="A13" s="44"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="46"/>
       <c r="D13" s="3">
         <v>12</v>
       </c>
@@ -3294,13 +3572,13 @@
         <v>27</v>
       </c>
       <c r="G13" s="4"/>
-      <c r="I13" s="48"/>
-      <c r="J13" s="48"/>
-      <c r="K13" s="48"/>
-      <c r="L13" s="48"/>
+      <c r="I13" s="50"/>
+      <c r="J13" s="50"/>
+      <c r="K13" s="50"/>
+      <c r="L13" s="50"/>
     </row>
     <row r="14" spans="1:12" ht="360" x14ac:dyDescent="0.25">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="40" t="s">
         <v>33</v>
       </c>
       <c r="B14">
@@ -3321,27 +3599,27 @@
       <c r="H14" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="I14" s="43" t="s">
+      <c r="I14" s="42" t="s">
         <v>491</v>
       </c>
-      <c r="J14" s="43" t="s">
+      <c r="J14" s="42" t="s">
         <v>493</v>
       </c>
-      <c r="K14" s="43" t="s">
+      <c r="K14" s="42" t="s">
         <v>492</v>
       </c>
-      <c r="L14" s="43" t="s">
+      <c r="L14" s="42" t="s">
         <v>494</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="330" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="50" t="s">
+      <c r="A15" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="54">
+      <c r="B15" s="47">
         <v>2018</v>
       </c>
-      <c r="C15" s="52" t="s">
+      <c r="C15" s="46" t="s">
         <v>40</v>
       </c>
       <c r="D15" s="3">
@@ -3350,7 +3628,7 @@
       <c r="E15" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="51" t="s">
+      <c r="F15" s="48" t="s">
         <v>46</v>
       </c>
       <c r="G15" s="4" t="s">
@@ -3359,61 +3637,61 @@
       <c r="H15" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="I15" s="48" t="s">
+      <c r="I15" s="50" t="s">
         <v>499</v>
       </c>
-      <c r="J15" s="49" t="s">
+      <c r="J15" s="51" t="s">
         <v>502</v>
       </c>
-      <c r="K15" s="48" t="s">
+      <c r="K15" s="50" t="s">
         <v>500</v>
       </c>
-      <c r="L15" s="48" t="s">
+      <c r="L15" s="50" t="s">
         <v>501</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="50"/>
-      <c r="B16" s="54"/>
-      <c r="C16" s="52"/>
+      <c r="A16" s="44"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="46"/>
       <c r="D16" s="3">
         <v>2</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F16" s="51"/>
+      <c r="F16" s="48"/>
       <c r="G16" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="I16" s="48"/>
-      <c r="J16" s="49"/>
-      <c r="K16" s="48"/>
-      <c r="L16" s="48"/>
+      <c r="I16" s="50"/>
+      <c r="J16" s="51"/>
+      <c r="K16" s="50"/>
+      <c r="L16" s="50"/>
     </row>
     <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="50"/>
-      <c r="B17" s="54"/>
-      <c r="C17" s="52"/>
+      <c r="A17" s="44"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="46"/>
       <c r="D17" s="3">
         <v>3</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F17" s="51"/>
+      <c r="F17" s="48"/>
       <c r="G17" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="I17" s="48"/>
-      <c r="J17" s="49"/>
-      <c r="K17" s="48"/>
-      <c r="L17" s="48"/>
+      <c r="I17" s="50"/>
+      <c r="J17" s="51"/>
+      <c r="K17" s="50"/>
+      <c r="L17" s="50"/>
     </row>
     <row r="18" spans="1:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="A18" s="50"/>
-      <c r="B18" s="54"/>
-      <c r="C18" s="52"/>
+      <c r="A18" s="44"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="46"/>
       <c r="D18" s="3">
         <v>4</v>
       </c>
@@ -3426,15 +3704,15 @@
       <c r="G18" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="I18" s="48"/>
-      <c r="J18" s="49"/>
-      <c r="K18" s="48"/>
-      <c r="L18" s="48"/>
+      <c r="I18" s="50"/>
+      <c r="J18" s="51"/>
+      <c r="K18" s="50"/>
+      <c r="L18" s="50"/>
     </row>
     <row r="19" spans="1:12" ht="96" x14ac:dyDescent="0.25">
-      <c r="A19" s="50"/>
-      <c r="B19" s="54"/>
-      <c r="C19" s="52"/>
+      <c r="A19" s="44"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="46"/>
       <c r="D19" s="3">
         <v>5</v>
       </c>
@@ -3447,15 +3725,15 @@
       <c r="G19" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="I19" s="48"/>
-      <c r="J19" s="49"/>
-      <c r="K19" s="48"/>
-      <c r="L19" s="48"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="50"/>
+      <c r="L19" s="50"/>
     </row>
     <row r="20" spans="1:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="A20" s="50"/>
-      <c r="B20" s="54"/>
-      <c r="C20" s="52"/>
+      <c r="A20" s="44"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="46"/>
       <c r="D20" s="3">
         <v>6</v>
       </c>
@@ -3465,15 +3743,15 @@
       <c r="F20" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="I20" s="48"/>
-      <c r="J20" s="49"/>
-      <c r="K20" s="48"/>
-      <c r="L20" s="48"/>
+      <c r="I20" s="50"/>
+      <c r="J20" s="51"/>
+      <c r="K20" s="50"/>
+      <c r="L20" s="50"/>
     </row>
     <row r="21" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A21" s="50"/>
-      <c r="B21" s="54"/>
-      <c r="C21" s="52"/>
+      <c r="A21" s="44"/>
+      <c r="B21" s="47"/>
+      <c r="C21" s="46"/>
       <c r="E21" s="4" t="s">
         <v>58</v>
       </c>
@@ -3483,13 +3761,13 @@
       <c r="G21" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="I21" s="48"/>
-      <c r="J21" s="49"/>
-      <c r="K21" s="48"/>
-      <c r="L21" s="48"/>
+      <c r="I21" s="50"/>
+      <c r="J21" s="51"/>
+      <c r="K21" s="50"/>
+      <c r="L21" s="50"/>
     </row>
     <row r="22" spans="1:12" ht="285" x14ac:dyDescent="0.25">
-      <c r="A22" s="41" t="s">
+      <c r="A22" s="40" t="s">
         <v>56</v>
       </c>
       <c r="B22">
@@ -3510,27 +3788,27 @@
       <c r="H22" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="I22" s="43" t="s">
+      <c r="I22" s="42" t="s">
         <v>495</v>
       </c>
-      <c r="J22" s="43" t="s">
+      <c r="J22" s="42" t="s">
         <v>496</v>
       </c>
-      <c r="K22" s="43" t="s">
+      <c r="K22" s="42" t="s">
         <v>497</v>
       </c>
-      <c r="L22" s="43" t="s">
+      <c r="L22" s="42" t="s">
         <v>498</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="390" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="50" t="s">
+      <c r="A23" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="B23" s="54">
+      <c r="B23" s="47">
         <v>2019</v>
       </c>
-      <c r="C23" s="52" t="s">
+      <c r="C23" s="46" t="s">
         <v>117</v>
       </c>
       <c r="E23" s="4" t="s">
@@ -3545,23 +3823,23 @@
       <c r="H23" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="I23" s="48" t="s">
+      <c r="I23" s="50" t="s">
         <v>503</v>
       </c>
-      <c r="J23" s="48" t="s">
+      <c r="J23" s="50" t="s">
         <v>505</v>
       </c>
-      <c r="K23" s="48" t="s">
+      <c r="K23" s="50" t="s">
         <v>268</v>
       </c>
-      <c r="L23" s="48" t="s">
+      <c r="L23" s="50" t="s">
         <v>504</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="50"/>
-      <c r="B24" s="54"/>
-      <c r="C24" s="52"/>
+      <c r="A24" s="44"/>
+      <c r="B24" s="47"/>
+      <c r="C24" s="46"/>
       <c r="E24" s="4" t="s">
         <v>63</v>
       </c>
@@ -3571,15 +3849,15 @@
       <c r="G24" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="I24" s="48"/>
-      <c r="J24" s="48"/>
-      <c r="K24" s="48"/>
-      <c r="L24" s="48"/>
+      <c r="I24" s="50"/>
+      <c r="J24" s="50"/>
+      <c r="K24" s="50"/>
+      <c r="L24" s="50"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="50"/>
-      <c r="B25" s="54"/>
-      <c r="C25" s="52"/>
+      <c r="A25" s="44"/>
+      <c r="B25" s="47"/>
+      <c r="C25" s="46"/>
       <c r="E25" s="4" t="s">
         <v>118</v>
       </c>
@@ -3589,15 +3867,15 @@
       <c r="G25" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="I25" s="48"/>
-      <c r="J25" s="48"/>
-      <c r="K25" s="48"/>
-      <c r="L25" s="48"/>
+      <c r="I25" s="50"/>
+      <c r="J25" s="50"/>
+      <c r="K25" s="50"/>
+      <c r="L25" s="50"/>
     </row>
     <row r="26" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="50"/>
-      <c r="B26" s="54"/>
-      <c r="C26" s="52"/>
+      <c r="A26" s="44"/>
+      <c r="B26" s="47"/>
+      <c r="C26" s="46"/>
       <c r="E26" s="4" t="s">
         <v>122</v>
       </c>
@@ -3607,15 +3885,15 @@
       <c r="G26" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="I26" s="48"/>
-      <c r="J26" s="48"/>
-      <c r="K26" s="48"/>
-      <c r="L26" s="48"/>
+      <c r="I26" s="50"/>
+      <c r="J26" s="50"/>
+      <c r="K26" s="50"/>
+      <c r="L26" s="50"/>
     </row>
     <row r="27" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="50"/>
-      <c r="B27" s="54"/>
-      <c r="C27" s="52"/>
+      <c r="A27" s="44"/>
+      <c r="B27" s="47"/>
+      <c r="C27" s="46"/>
       <c r="E27" s="4" t="s">
         <v>45</v>
       </c>
@@ -3625,19 +3903,19 @@
       <c r="G27" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="I27" s="48"/>
-      <c r="J27" s="48"/>
-      <c r="K27" s="48"/>
-      <c r="L27" s="48"/>
+      <c r="I27" s="50"/>
+      <c r="J27" s="50"/>
+      <c r="K27" s="50"/>
+      <c r="L27" s="50"/>
     </row>
     <row r="28" spans="1:12" ht="345" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="50" t="s">
+      <c r="A28" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="B28" s="55">
+      <c r="B28" s="45">
         <v>2021</v>
       </c>
-      <c r="C28" s="52" t="s">
+      <c r="C28" s="46" t="s">
         <v>67</v>
       </c>
       <c r="E28" s="4" t="s">
@@ -3649,26 +3927,26 @@
       <c r="G28" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="H28" s="52" t="s">
+      <c r="H28" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="I28" s="48" t="s">
+      <c r="I28" s="50" t="s">
+        <v>547</v>
+      </c>
+      <c r="J28" s="50" t="s">
+        <v>548</v>
+      </c>
+      <c r="K28" s="50" t="s">
         <v>549</v>
       </c>
-      <c r="J28" s="48" t="s">
+      <c r="L28" s="50" t="s">
         <v>550</v>
       </c>
-      <c r="K28" s="48" t="s">
-        <v>551</v>
-      </c>
-      <c r="L28" s="48" t="s">
-        <v>552</v>
-      </c>
     </row>
     <row r="29" spans="1:12" ht="120" x14ac:dyDescent="0.25">
-      <c r="A29" s="50"/>
-      <c r="B29" s="55"/>
-      <c r="C29" s="52"/>
+      <c r="A29" s="44"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="46"/>
       <c r="E29" s="4" t="s">
         <v>69</v>
       </c>
@@ -3678,16 +3956,16 @@
       <c r="G29" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="H29" s="52"/>
-      <c r="I29" s="48"/>
-      <c r="J29" s="48"/>
-      <c r="K29" s="48"/>
-      <c r="L29" s="48"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="50"/>
+      <c r="K29" s="50"/>
+      <c r="L29" s="50"/>
     </row>
     <row r="30" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="50"/>
-      <c r="B30" s="55"/>
-      <c r="C30" s="52"/>
+      <c r="A30" s="44"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="46"/>
       <c r="E30" s="4" t="s">
         <v>70</v>
       </c>
@@ -3697,14 +3975,14 @@
       <c r="G30" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="H30" s="52"/>
-      <c r="I30" s="48"/>
-      <c r="J30" s="48"/>
-      <c r="K30" s="48"/>
-      <c r="L30" s="48"/>
+      <c r="H30" s="46"/>
+      <c r="I30" s="50"/>
+      <c r="J30" s="50"/>
+      <c r="K30" s="50"/>
+      <c r="L30" s="50"/>
     </row>
     <row r="31" spans="1:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="50" t="s">
+      <c r="A31" s="44" t="s">
         <v>78</v>
       </c>
       <c r="B31">
@@ -3719,21 +3997,21 @@
       <c r="F31" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I31" s="48" t="s">
+      <c r="I31" s="50" t="s">
+        <v>534</v>
+      </c>
+      <c r="J31" s="50" t="s">
+        <v>535</v>
+      </c>
+      <c r="K31" s="50" t="s">
         <v>536</v>
       </c>
-      <c r="J31" s="48" t="s">
-        <v>537</v>
-      </c>
-      <c r="K31" s="48" t="s">
-        <v>538</v>
-      </c>
-      <c r="L31" s="48" t="s">
-        <v>543</v>
+      <c r="L31" s="50" t="s">
+        <v>541</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="105" x14ac:dyDescent="0.25">
-      <c r="A32" s="50"/>
+      <c r="A32" s="44"/>
       <c r="E32" s="4" t="s">
         <v>82</v>
       </c>
@@ -3746,13 +4024,13 @@
       <c r="H32" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="I32" s="48"/>
-      <c r="J32" s="48"/>
-      <c r="K32" s="48"/>
-      <c r="L32" s="48"/>
+      <c r="I32" s="50"/>
+      <c r="J32" s="50"/>
+      <c r="K32" s="50"/>
+      <c r="L32" s="50"/>
     </row>
     <row r="33" spans="1:12" ht="105" x14ac:dyDescent="0.25">
-      <c r="A33" s="50"/>
+      <c r="A33" s="44"/>
       <c r="E33" s="4" t="s">
         <v>83</v>
       </c>
@@ -3762,13 +4040,13 @@
       <c r="G33" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I33" s="48"/>
-      <c r="J33" s="48"/>
-      <c r="K33" s="48"/>
-      <c r="L33" s="48"/>
+      <c r="I33" s="50"/>
+      <c r="J33" s="50"/>
+      <c r="K33" s="50"/>
+      <c r="L33" s="50"/>
     </row>
     <row r="34" spans="1:12" ht="126" x14ac:dyDescent="0.25">
-      <c r="A34" s="50"/>
+      <c r="A34" s="44"/>
       <c r="E34" s="4" t="s">
         <v>70</v>
       </c>
@@ -3778,26 +4056,26 @@
       <c r="G34" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="I34" s="48"/>
-      <c r="J34" s="48"/>
-      <c r="K34" s="48"/>
-      <c r="L34" s="48"/>
+      <c r="I34" s="50"/>
+      <c r="J34" s="50"/>
+      <c r="K34" s="50"/>
+      <c r="L34" s="50"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="50"/>
+      <c r="A35" s="44"/>
       <c r="E35" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I35" s="48"/>
-      <c r="J35" s="48"/>
-      <c r="K35" s="48"/>
-      <c r="L35" s="48"/>
+      <c r="I35" s="50"/>
+      <c r="J35" s="50"/>
+      <c r="K35" s="50"/>
+      <c r="L35" s="50"/>
     </row>
     <row r="36" spans="1:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="50" t="s">
+      <c r="A36" s="44" t="s">
         <v>39</v>
       </c>
       <c r="B36">
@@ -3813,34 +4091,34 @@
       <c r="H36" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="I36" s="48" t="s">
+      <c r="I36" s="50" t="s">
+        <v>538</v>
+      </c>
+      <c r="J36" s="50" t="s">
+        <v>539</v>
+      </c>
+      <c r="K36" s="50" t="s">
         <v>540</v>
       </c>
-      <c r="J36" s="48" t="s">
-        <v>541</v>
-      </c>
-      <c r="K36" s="48" t="s">
+      <c r="L36" s="50" t="s">
         <v>542</v>
       </c>
-      <c r="L36" s="48" t="s">
-        <v>544</v>
-      </c>
     </row>
     <row r="37" spans="1:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="A37" s="50"/>
+      <c r="A37" s="44"/>
       <c r="E37" s="5" t="s">
         <v>92</v>
       </c>
       <c r="G37" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="I37" s="48"/>
-      <c r="J37" s="48"/>
-      <c r="K37" s="48"/>
-      <c r="L37" s="48"/>
+      <c r="I37" s="50"/>
+      <c r="J37" s="50"/>
+      <c r="K37" s="50"/>
+      <c r="L37" s="50"/>
     </row>
     <row r="38" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A38" s="50"/>
+      <c r="A38" s="44"/>
       <c r="E38" s="5" t="s">
         <v>93</v>
       </c>
@@ -3850,24 +4128,24 @@
       <c r="G38" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="I38" s="48"/>
-      <c r="J38" s="48"/>
-      <c r="K38" s="48"/>
-      <c r="L38" s="48"/>
+      <c r="I38" s="50"/>
+      <c r="J38" s="50"/>
+      <c r="K38" s="50"/>
+      <c r="L38" s="50"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="50"/>
+      <c r="A39" s="44"/>
       <c r="E39" s="5" t="s">
         <v>94</v>
       </c>
       <c r="F39" s="4"/>
-      <c r="I39" s="48"/>
-      <c r="J39" s="48"/>
-      <c r="K39" s="48"/>
-      <c r="L39" s="48"/>
+      <c r="I39" s="50"/>
+      <c r="J39" s="50"/>
+      <c r="K39" s="50"/>
+      <c r="L39" s="50"/>
     </row>
     <row r="40" spans="1:12" ht="105" x14ac:dyDescent="0.25">
-      <c r="A40" s="50"/>
+      <c r="A40" s="44"/>
       <c r="E40" s="5" t="s">
         <v>95</v>
       </c>
@@ -3877,24 +4155,24 @@
       <c r="G40" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="I40" s="48"/>
-      <c r="J40" s="48"/>
-      <c r="K40" s="48"/>
-      <c r="L40" s="48"/>
+      <c r="I40" s="50"/>
+      <c r="J40" s="50"/>
+      <c r="K40" s="50"/>
+      <c r="L40" s="50"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="50"/>
+      <c r="A41" s="44"/>
       <c r="E41" s="5" t="s">
         <v>16</v>
       </c>
       <c r="F41" s="4"/>
-      <c r="I41" s="48"/>
-      <c r="J41" s="48"/>
-      <c r="K41" s="48"/>
-      <c r="L41" s="48"/>
+      <c r="I41" s="50"/>
+      <c r="J41" s="50"/>
+      <c r="K41" s="50"/>
+      <c r="L41" s="50"/>
     </row>
     <row r="42" spans="1:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="50" t="s">
+      <c r="A42" s="44" t="s">
         <v>102</v>
       </c>
       <c r="B42">
@@ -3915,21 +4193,21 @@
       <c r="H42" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="I42" s="48" t="s">
+      <c r="I42" s="50" t="s">
+        <v>543</v>
+      </c>
+      <c r="J42" s="50" t="s">
+        <v>544</v>
+      </c>
+      <c r="K42" s="50" t="s">
         <v>545</v>
       </c>
-      <c r="J42" s="48" t="s">
+      <c r="L42" s="50" t="s">
         <v>546</v>
       </c>
-      <c r="K42" s="48" t="s">
-        <v>547</v>
-      </c>
-      <c r="L42" s="48" t="s">
-        <v>548</v>
-      </c>
     </row>
     <row r="43" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A43" s="50"/>
+      <c r="A43" s="44"/>
       <c r="E43" s="4" t="s">
         <v>105</v>
       </c>
@@ -3939,13 +4217,13 @@
       <c r="G43" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="I43" s="48"/>
-      <c r="J43" s="48"/>
-      <c r="K43" s="48"/>
-      <c r="L43" s="48"/>
+      <c r="I43" s="50"/>
+      <c r="J43" s="50"/>
+      <c r="K43" s="50"/>
+      <c r="L43" s="50"/>
     </row>
     <row r="44" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A44" s="50"/>
+      <c r="A44" s="44"/>
       <c r="E44" s="4" t="s">
         <v>106</v>
       </c>
@@ -3955,13 +4233,13 @@
       <c r="G44" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="I44" s="48"/>
-      <c r="J44" s="48"/>
-      <c r="K44" s="48"/>
-      <c r="L44" s="48"/>
+      <c r="I44" s="50"/>
+      <c r="J44" s="50"/>
+      <c r="K44" s="50"/>
+      <c r="L44" s="50"/>
     </row>
     <row r="45" spans="1:12" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="50"/>
+      <c r="A45" s="44"/>
       <c r="E45" s="4" t="s">
         <v>107</v>
       </c>
@@ -3971,13 +4249,13 @@
       <c r="G45" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="I45" s="48"/>
-      <c r="J45" s="48"/>
-      <c r="K45" s="48"/>
-      <c r="L45" s="48"/>
+      <c r="I45" s="50"/>
+      <c r="J45" s="50"/>
+      <c r="K45" s="50"/>
+      <c r="L45" s="50"/>
     </row>
     <row r="46" spans="1:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="50" t="s">
+      <c r="A46" s="44" t="s">
         <v>280</v>
       </c>
       <c r="B46">
@@ -3998,21 +4276,21 @@
       <c r="H46" s="3" t="s">
         <v>329</v>
       </c>
-      <c r="I46" s="48" t="s">
+      <c r="I46" s="50" t="s">
         <v>506</v>
       </c>
-      <c r="J46" s="48" t="s">
+      <c r="J46" s="50" t="s">
         <v>507</v>
       </c>
-      <c r="K46" s="48" t="s">
-        <v>510</v>
-      </c>
-      <c r="L46" s="48" t="s">
-        <v>553</v>
+      <c r="K46" s="50" t="s">
+        <v>508</v>
+      </c>
+      <c r="L46" s="50" t="s">
+        <v>551</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="50"/>
+      <c r="A47" s="44"/>
       <c r="E47" s="4" t="s">
         <v>292</v>
       </c>
@@ -4022,13 +4300,13 @@
       <c r="G47" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="I47" s="48"/>
-      <c r="J47" s="48"/>
-      <c r="K47" s="48"/>
-      <c r="L47" s="48"/>
+      <c r="I47" s="50"/>
+      <c r="J47" s="50"/>
+      <c r="K47" s="50"/>
+      <c r="L47" s="50"/>
     </row>
     <row r="48" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A48" s="50"/>
+      <c r="A48" s="44"/>
       <c r="E48" s="4" t="s">
         <v>93</v>
       </c>
@@ -4038,13 +4316,13 @@
       <c r="G48" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="I48" s="48"/>
-      <c r="J48" s="48"/>
-      <c r="K48" s="48"/>
-      <c r="L48" s="48"/>
+      <c r="I48" s="50"/>
+      <c r="J48" s="50"/>
+      <c r="K48" s="50"/>
+      <c r="L48" s="50"/>
     </row>
     <row r="49" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="50"/>
+      <c r="A49" s="44"/>
       <c r="E49" s="4" t="s">
         <v>284</v>
       </c>
@@ -4054,13 +4332,13 @@
       <c r="G49" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="I49" s="48"/>
-      <c r="J49" s="48"/>
-      <c r="K49" s="48"/>
-      <c r="L49" s="48"/>
+      <c r="I49" s="50"/>
+      <c r="J49" s="50"/>
+      <c r="K49" s="50"/>
+      <c r="L49" s="50"/>
     </row>
     <row r="50" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A50" s="50"/>
+      <c r="A50" s="44"/>
       <c r="E50" s="4" t="s">
         <v>285</v>
       </c>
@@ -4070,13 +4348,13 @@
       <c r="G50" s="4" t="s">
         <v>334</v>
       </c>
-      <c r="I50" s="48"/>
-      <c r="J50" s="48"/>
-      <c r="K50" s="48"/>
-      <c r="L50" s="48"/>
+      <c r="I50" s="50"/>
+      <c r="J50" s="50"/>
+      <c r="K50" s="50"/>
+      <c r="L50" s="50"/>
     </row>
     <row r="51" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="50"/>
+      <c r="A51" s="44"/>
       <c r="C51" s="36"/>
       <c r="E51" s="4" t="s">
         <v>330</v>
@@ -4087,13 +4365,13 @@
       <c r="G51" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="I51" s="48"/>
-      <c r="J51" s="48"/>
-      <c r="K51" s="48"/>
-      <c r="L51" s="48"/>
+      <c r="I51" s="50"/>
+      <c r="J51" s="50"/>
+      <c r="K51" s="50"/>
+      <c r="L51" s="50"/>
     </row>
     <row r="52" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A52" s="50"/>
+      <c r="A52" s="44"/>
       <c r="E52" s="4" t="s">
         <v>70</v>
       </c>
@@ -4103,48 +4381,13 @@
       <c r="G52" s="4" t="s">
         <v>335</v>
       </c>
-      <c r="I52" s="48"/>
-      <c r="J52" s="48"/>
-      <c r="K52" s="48"/>
-      <c r="L52" s="48"/>
+      <c r="I52" s="50"/>
+      <c r="J52" s="50"/>
+      <c r="K52" s="50"/>
+      <c r="L52" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="H28:H30"/>
-    <mergeCell ref="C23:C27"/>
-    <mergeCell ref="B23:B27"/>
-    <mergeCell ref="A23:A27"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="C2:C13"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="C15:C21"/>
-    <mergeCell ref="B15:B21"/>
-    <mergeCell ref="A15:A21"/>
-    <mergeCell ref="A31:A35"/>
-    <mergeCell ref="A36:A41"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="A46:A52"/>
-    <mergeCell ref="I46:I52"/>
-    <mergeCell ref="I42:I45"/>
-    <mergeCell ref="I36:I41"/>
-    <mergeCell ref="I31:I35"/>
-    <mergeCell ref="I28:I30"/>
-    <mergeCell ref="I23:I27"/>
-    <mergeCell ref="I15:I21"/>
-    <mergeCell ref="I2:I13"/>
-    <mergeCell ref="J46:J52"/>
-    <mergeCell ref="J42:J45"/>
-    <mergeCell ref="J36:J41"/>
-    <mergeCell ref="J31:J35"/>
-    <mergeCell ref="J28:J30"/>
-    <mergeCell ref="J23:J27"/>
-    <mergeCell ref="J15:J21"/>
-    <mergeCell ref="J2:J13"/>
     <mergeCell ref="K23:K27"/>
     <mergeCell ref="K15:K21"/>
     <mergeCell ref="K2:K13"/>
@@ -4161,6 +4404,41 @@
     <mergeCell ref="K36:K41"/>
     <mergeCell ref="K31:K35"/>
     <mergeCell ref="K28:K30"/>
+    <mergeCell ref="I28:I30"/>
+    <mergeCell ref="I23:I27"/>
+    <mergeCell ref="I15:I21"/>
+    <mergeCell ref="I2:I13"/>
+    <mergeCell ref="J46:J52"/>
+    <mergeCell ref="J42:J45"/>
+    <mergeCell ref="J36:J41"/>
+    <mergeCell ref="J31:J35"/>
+    <mergeCell ref="J28:J30"/>
+    <mergeCell ref="J23:J27"/>
+    <mergeCell ref="J15:J21"/>
+    <mergeCell ref="J2:J13"/>
+    <mergeCell ref="A31:A35"/>
+    <mergeCell ref="A36:A41"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="A46:A52"/>
+    <mergeCell ref="I46:I52"/>
+    <mergeCell ref="I42:I45"/>
+    <mergeCell ref="I36:I41"/>
+    <mergeCell ref="I31:I35"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="C2:C13"/>
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="C15:C21"/>
+    <mergeCell ref="B15:B21"/>
+    <mergeCell ref="A15:A21"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="H28:H30"/>
+    <mergeCell ref="C23:C27"/>
+    <mergeCell ref="B23:B27"/>
+    <mergeCell ref="A23:A27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4203,7 +4481,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="53" t="s">
         <v>132</v>
       </c>
       <c r="B2" s="22" t="s">
@@ -4220,7 +4498,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="57"/>
+      <c r="A3" s="53"/>
       <c r="B3" s="22" t="s">
         <v>142</v>
       </c>
@@ -4235,7 +4513,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="57"/>
+      <c r="A4" s="53"/>
       <c r="B4" s="22" t="s">
         <v>143</v>
       </c>
@@ -4250,7 +4528,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="57"/>
+      <c r="A5" s="53"/>
       <c r="B5" s="22" t="s">
         <v>146</v>
       </c>
@@ -4265,7 +4543,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="57"/>
+      <c r="A6" s="53"/>
       <c r="B6" s="22" t="s">
         <v>180</v>
       </c>
@@ -4277,7 +4555,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="57"/>
+      <c r="A7" s="53"/>
       <c r="B7" s="22" t="s">
         <v>187</v>
       </c>
@@ -4289,7 +4567,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="57"/>
+      <c r="A8" s="53"/>
       <c r="B8" s="22" t="s">
         <v>188</v>
       </c>
@@ -4301,7 +4579,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="57"/>
+      <c r="A9" s="53"/>
       <c r="C9" s="23" t="s">
         <v>147</v>
       </c>
@@ -4310,7 +4588,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="57"/>
+      <c r="A10" s="53"/>
       <c r="C10" s="23" t="s">
         <v>147</v>
       </c>
@@ -4319,7 +4597,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="57"/>
+      <c r="A11" s="53"/>
       <c r="C11" s="23" t="s">
         <v>148</v>
       </c>
@@ -4328,7 +4606,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="57"/>
+      <c r="A12" s="53"/>
       <c r="C12" s="23" t="s">
         <v>158</v>
       </c>
@@ -4337,7 +4615,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="165" x14ac:dyDescent="0.25">
-      <c r="A13" s="57"/>
+      <c r="A13" s="53"/>
       <c r="C13" s="23" t="s">
         <v>159</v>
       </c>
@@ -4346,7 +4624,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="57"/>
+      <c r="A14" s="53"/>
       <c r="C14" s="23" t="s">
         <v>160</v>
       </c>
@@ -4355,7 +4633,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="57"/>
+      <c r="A15" s="53"/>
       <c r="C15" s="23" t="s">
         <v>163</v>
       </c>
@@ -4364,7 +4642,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="57"/>
+      <c r="A16" s="53"/>
       <c r="C16" s="23" t="s">
         <v>174</v>
       </c>
@@ -4373,7 +4651,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A17" s="57"/>
+      <c r="A17" s="53"/>
       <c r="C17" s="23" t="s">
         <v>179</v>
       </c>
@@ -4382,7 +4660,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="57"/>
+      <c r="A18" s="53"/>
       <c r="C18" s="23" t="s">
         <v>186</v>
       </c>
@@ -4391,92 +4669,92 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A19" s="57"/>
+      <c r="A19" s="53"/>
       <c r="E19" s="25" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="165" x14ac:dyDescent="0.25">
-      <c r="A20" s="57"/>
+      <c r="A20" s="53"/>
       <c r="E20" s="25" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="135" x14ac:dyDescent="0.25">
-      <c r="A21" s="57"/>
+      <c r="A21" s="53"/>
       <c r="E21" s="25" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="57"/>
+      <c r="A22" s="53"/>
       <c r="E22" s="25" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="57"/>
+      <c r="A23" s="53"/>
       <c r="E23" s="25" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="57"/>
+      <c r="A24" s="53"/>
       <c r="E24" s="25" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="57"/>
+      <c r="A25" s="53"/>
       <c r="E25" s="25" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="57"/>
+      <c r="A26" s="53"/>
       <c r="E26" s="25" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="135" x14ac:dyDescent="0.25">
-      <c r="A27" s="57"/>
+      <c r="A27" s="53"/>
       <c r="E27" s="25" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A28" s="57"/>
+      <c r="A28" s="53"/>
       <c r="E28" s="25" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A29" s="57"/>
+      <c r="A29" s="53"/>
       <c r="E29" s="25" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="135" x14ac:dyDescent="0.25">
-      <c r="A30" s="57"/>
+      <c r="A30" s="53"/>
       <c r="E30" s="25" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A31" s="57"/>
+      <c r="A31" s="53"/>
       <c r="E31" s="25" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A32" s="59"/>
+      <c r="A32" s="55"/>
       <c r="B32" s="31"/>
       <c r="E32" s="27" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="150" x14ac:dyDescent="0.25">
-      <c r="A33" s="56" t="s">
+      <c r="A33" s="52" t="s">
         <v>189</v>
       </c>
       <c r="B33" s="30" t="s">
@@ -4493,7 +4771,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A34" s="57"/>
+      <c r="A34" s="53"/>
       <c r="B34" s="22" t="s">
         <v>210</v>
       </c>
@@ -4508,7 +4786,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="57"/>
+      <c r="A35" s="53"/>
       <c r="C35" s="23" t="s">
         <v>195</v>
       </c>
@@ -4520,7 +4798,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="57"/>
+      <c r="A36" s="53"/>
       <c r="C36" s="23" t="s">
         <v>196</v>
       </c>
@@ -4529,7 +4807,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A37" s="57"/>
+      <c r="A37" s="53"/>
       <c r="C37" s="23" t="s">
         <v>197</v>
       </c>
@@ -4538,7 +4816,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="57"/>
+      <c r="A38" s="53"/>
       <c r="C38" s="23" t="s">
         <v>203</v>
       </c>
@@ -4547,7 +4825,7 @@
       </c>
     </row>
     <row r="39" spans="1:5" ht="180" x14ac:dyDescent="0.25">
-      <c r="A39" s="57"/>
+      <c r="A39" s="53"/>
       <c r="C39" s="23" t="s">
         <v>204</v>
       </c>
@@ -4556,26 +4834,26 @@
       </c>
     </row>
     <row r="40" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A40" s="57"/>
+      <c r="A40" s="53"/>
       <c r="E40" s="25" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" s="57"/>
+      <c r="A41" s="53"/>
       <c r="E41" s="25" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="59"/>
+      <c r="A42" s="55"/>
       <c r="D42" s="33"/>
       <c r="E42" s="27" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="300" x14ac:dyDescent="0.25">
-      <c r="A43" s="56" t="s">
+      <c r="A43" s="52" t="s">
         <v>211</v>
       </c>
       <c r="B43" s="32"/>
@@ -4590,7 +4868,7 @@
       </c>
     </row>
     <row r="44" spans="1:5" ht="180" x14ac:dyDescent="0.25">
-      <c r="A44" s="58"/>
+      <c r="A44" s="54"/>
       <c r="C44" s="23" t="s">
         <v>214</v>
       </c>
@@ -4599,14 +4877,14 @@
       </c>
     </row>
     <row r="45" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="58"/>
+      <c r="A45" s="54"/>
       <c r="B45" s="31"/>
       <c r="C45" s="34" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A46" s="56" t="s">
+      <c r="A46" s="52" t="s">
         <v>218</v>
       </c>
       <c r="B46" s="22" t="s">
@@ -4623,7 +4901,7 @@
       </c>
     </row>
     <row r="47" spans="1:5" ht="165" x14ac:dyDescent="0.25">
-      <c r="A47" s="57"/>
+      <c r="A47" s="53"/>
       <c r="B47" s="22" t="s">
         <v>221</v>
       </c>
@@ -4638,7 +4916,7 @@
       </c>
     </row>
     <row r="48" spans="1:5" ht="135" x14ac:dyDescent="0.25">
-      <c r="A48" s="57"/>
+      <c r="A48" s="53"/>
       <c r="B48" s="22" t="s">
         <v>222</v>
       </c>
@@ -4650,7 +4928,7 @@
       </c>
     </row>
     <row r="49" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A49" s="57"/>
+      <c r="A49" s="53"/>
       <c r="B49" s="22" t="s">
         <v>224</v>
       </c>
@@ -4662,7 +4940,7 @@
       </c>
     </row>
     <row r="50" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A50" s="57"/>
+      <c r="A50" s="53"/>
       <c r="B50" s="22" t="s">
         <v>248</v>
       </c>
@@ -4674,7 +4952,7 @@
       </c>
     </row>
     <row r="51" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A51" s="57"/>
+      <c r="A51" s="53"/>
       <c r="B51" s="22" t="s">
         <v>250</v>
       </c>
@@ -4686,7 +4964,7 @@
       </c>
     </row>
     <row r="52" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A52" s="57"/>
+      <c r="A52" s="53"/>
       <c r="B52" s="22" t="s">
         <v>252</v>
       </c>
@@ -4698,7 +4976,7 @@
       </c>
     </row>
     <row r="53" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A53" s="57"/>
+      <c r="A53" s="53"/>
       <c r="B53" s="22" t="s">
         <v>253</v>
       </c>
@@ -4710,7 +4988,7 @@
       </c>
     </row>
     <row r="54" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A54" s="57"/>
+      <c r="A54" s="53"/>
       <c r="B54" s="22" t="s">
         <v>258</v>
       </c>
@@ -4722,7 +5000,7 @@
       </c>
     </row>
     <row r="55" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A55" s="57"/>
+      <c r="A55" s="53"/>
       <c r="B55" s="22" t="s">
         <v>259</v>
       </c>
@@ -4731,7 +5009,7 @@
       </c>
     </row>
     <row r="56" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A56" s="57"/>
+      <c r="A56" s="53"/>
       <c r="B56" s="22" t="s">
         <v>261</v>
       </c>
@@ -4740,7 +5018,7 @@
       </c>
     </row>
     <row r="57" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A57" s="57"/>
+      <c r="A57" s="53"/>
       <c r="B57" s="22" t="s">
         <v>262</v>
       </c>
@@ -4749,7 +5027,7 @@
       </c>
     </row>
     <row r="58" spans="1:5" ht="165" x14ac:dyDescent="0.25">
-      <c r="A58" s="57"/>
+      <c r="A58" s="53"/>
       <c r="B58" s="22" t="s">
         <v>263</v>
       </c>
@@ -4758,7 +5036,7 @@
       </c>
     </row>
     <row r="59" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A59" s="57"/>
+      <c r="A59" s="53"/>
       <c r="B59" s="22" t="s">
         <v>265</v>
       </c>
@@ -4767,56 +5045,56 @@
       </c>
     </row>
     <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="57"/>
+      <c r="A60" s="53"/>
       <c r="E60" s="25" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A61" s="57"/>
+      <c r="A61" s="53"/>
       <c r="E61" s="25" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A62" s="57"/>
+      <c r="A62" s="53"/>
       <c r="E62" s="25" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="57"/>
+      <c r="A63" s="53"/>
       <c r="E63" s="25" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A64" s="57"/>
+      <c r="A64" s="53"/>
       <c r="E64" s="25" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A65" s="57"/>
+      <c r="A65" s="53"/>
       <c r="E65" s="25" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A66" s="57"/>
+      <c r="A66" s="53"/>
       <c r="E66" s="25" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A67" s="57"/>
+      <c r="A67" s="53"/>
       <c r="B67" s="31"/>
       <c r="E67" s="25" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="210" x14ac:dyDescent="0.25">
-      <c r="A68" s="56" t="s">
+      <c r="A68" s="52" t="s">
         <v>267</v>
       </c>
       <c r="B68" s="22" t="s">
@@ -4833,7 +5111,7 @@
       </c>
     </row>
     <row r="69" spans="1:5" ht="255" x14ac:dyDescent="0.25">
-      <c r="A69" s="57"/>
+      <c r="A69" s="53"/>
       <c r="B69" s="22" t="s">
         <v>269</v>
       </c>
@@ -4845,7 +5123,7 @@
       </c>
     </row>
     <row r="70" spans="1:5" ht="315" x14ac:dyDescent="0.25">
-      <c r="A70" s="57"/>
+      <c r="A70" s="53"/>
       <c r="B70" s="22" t="s">
         <v>277</v>
       </c>
@@ -4857,13 +5135,13 @@
       </c>
     </row>
     <row r="71" spans="1:5" ht="360" x14ac:dyDescent="0.25">
-      <c r="A71" s="57"/>
+      <c r="A71" s="53"/>
       <c r="C71" s="23" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A72" s="59"/>
+      <c r="A72" s="55"/>
       <c r="B72" s="31"/>
       <c r="C72" s="34" t="s">
         <v>278</v>
@@ -4871,7 +5149,7 @@
       <c r="D72" s="33"/>
     </row>
     <row r="73" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A73" s="56" t="s">
+      <c r="A73" s="52" t="s">
         <v>279</v>
       </c>
       <c r="B73" s="22" t="s">
@@ -4888,7 +5166,7 @@
       </c>
     </row>
     <row r="74" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A74" s="58"/>
+      <c r="A74" s="54"/>
       <c r="B74" s="22" t="s">
         <v>282</v>
       </c>
@@ -4903,7 +5181,7 @@
       </c>
     </row>
     <row r="75" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A75" s="58"/>
+      <c r="A75" s="54"/>
       <c r="B75" s="22" t="s">
         <v>325</v>
       </c>
@@ -4918,7 +5196,7 @@
       </c>
     </row>
     <row r="76" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A76" s="58"/>
+      <c r="A76" s="54"/>
       <c r="B76" s="22" t="s">
         <v>326</v>
       </c>
@@ -4933,7 +5211,7 @@
       </c>
     </row>
     <row r="77" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A77" s="58"/>
+      <c r="A77" s="54"/>
       <c r="B77" s="22" t="s">
         <v>327</v>
       </c>
@@ -4948,7 +5226,7 @@
       </c>
     </row>
     <row r="78" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A78" s="58"/>
+      <c r="A78" s="54"/>
       <c r="C78" s="23" t="s">
         <v>313</v>
       </c>
@@ -4960,7 +5238,7 @@
       </c>
     </row>
     <row r="79" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A79" s="58"/>
+      <c r="A79" s="54"/>
       <c r="C79" s="23" t="s">
         <v>316</v>
       </c>
@@ -4972,7 +5250,7 @@
       </c>
     </row>
     <row r="80" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A80" s="58"/>
+      <c r="A80" s="54"/>
       <c r="C80" s="23" t="s">
         <v>317</v>
       </c>
@@ -4984,7 +5262,7 @@
       </c>
     </row>
     <row r="81" spans="1:5" ht="135" x14ac:dyDescent="0.25">
-      <c r="A81" s="58"/>
+      <c r="A81" s="54"/>
       <c r="C81" s="23" t="s">
         <v>319</v>
       </c>
@@ -4996,7 +5274,7 @@
       </c>
     </row>
     <row r="82" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A82" s="58"/>
+      <c r="A82" s="54"/>
       <c r="C82" s="23" t="s">
         <v>320</v>
       </c>
@@ -5008,7 +5286,7 @@
       </c>
     </row>
     <row r="83" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A83" s="58"/>
+      <c r="A83" s="54"/>
       <c r="C83" s="34" t="s">
         <v>328</v>
       </c>
@@ -5016,7 +5294,7 @@
       <c r="E83" s="27"/>
     </row>
     <row r="84" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A84" s="56" t="s">
+      <c r="A84" s="52" t="s">
         <v>337</v>
       </c>
       <c r="B84" s="32" t="s">
@@ -5033,7 +5311,7 @@
       </c>
     </row>
     <row r="85" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A85" s="57"/>
+      <c r="A85" s="53"/>
       <c r="B85" s="22" t="s">
         <v>341</v>
       </c>
@@ -5048,7 +5326,7 @@
       </c>
     </row>
     <row r="86" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A86" s="57"/>
+      <c r="A86" s="53"/>
       <c r="B86" s="22" t="s">
         <v>368</v>
       </c>
@@ -5063,7 +5341,7 @@
       </c>
     </row>
     <row r="87" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A87" s="57"/>
+      <c r="A87" s="53"/>
       <c r="B87" s="22" t="s">
         <v>370</v>
       </c>
@@ -5075,7 +5353,7 @@
       </c>
     </row>
     <row r="88" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A88" s="57"/>
+      <c r="A88" s="53"/>
       <c r="B88" s="22" t="s">
         <v>381</v>
       </c>
@@ -5087,7 +5365,7 @@
       </c>
     </row>
     <row r="89" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A89" s="57"/>
+      <c r="A89" s="53"/>
       <c r="C89" s="23" t="s">
         <v>369</v>
       </c>
@@ -5096,7 +5374,7 @@
       </c>
     </row>
     <row r="90" spans="1:5" ht="135" x14ac:dyDescent="0.25">
-      <c r="A90" s="57"/>
+      <c r="A90" s="53"/>
       <c r="C90" s="23" t="s">
         <v>371</v>
       </c>
@@ -5105,16 +5383,16 @@
       </c>
     </row>
     <row r="91" spans="1:5" ht="225" x14ac:dyDescent="0.25">
-      <c r="A91" s="57"/>
+      <c r="A91" s="53"/>
       <c r="C91" s="23" t="s">
         <v>372</v>
       </c>
       <c r="E91" s="25" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A92" s="57"/>
+      <c r="A92" s="53"/>
       <c r="C92" s="23" t="s">
         <v>373</v>
       </c>
@@ -5123,7 +5401,7 @@
       </c>
     </row>
     <row r="93" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A93" s="57"/>
+      <c r="A93" s="53"/>
       <c r="C93" s="23" t="s">
         <v>375</v>
       </c>
@@ -5132,7 +5410,7 @@
       </c>
     </row>
     <row r="94" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A94" s="57"/>
+      <c r="A94" s="53"/>
       <c r="C94" s="23" t="s">
         <v>377</v>
       </c>
@@ -5141,7 +5419,7 @@
       </c>
     </row>
     <row r="95" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A95" s="57"/>
+      <c r="A95" s="53"/>
       <c r="C95" s="23" t="s">
         <v>382</v>
       </c>
@@ -5150,98 +5428,98 @@
       </c>
     </row>
     <row r="96" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A96" s="57"/>
+      <c r="A96" s="53"/>
       <c r="E96" s="25" t="s">
         <v>353</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A97" s="57"/>
+      <c r="A97" s="53"/>
       <c r="E97" s="25" t="s">
         <v>354</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A98" s="57"/>
+      <c r="A98" s="53"/>
       <c r="E98" s="25" t="s">
         <v>355</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A99" s="57"/>
+      <c r="A99" s="53"/>
       <c r="E99" s="25" t="s">
         <v>357</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A100" s="57"/>
+      <c r="A100" s="53"/>
       <c r="E100" s="25" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="57"/>
+      <c r="A101" s="53"/>
       <c r="E101" s="25" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A102" s="57"/>
+      <c r="A102" s="53"/>
       <c r="E102" s="25" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A103" s="57"/>
+      <c r="A103" s="53"/>
       <c r="E103" s="25" t="s">
         <v>362</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A104" s="57"/>
+      <c r="A104" s="53"/>
       <c r="E104" s="25" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A105" s="57"/>
+      <c r="A105" s="53"/>
       <c r="E105" s="25" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A106" s="57"/>
+      <c r="A106" s="53"/>
       <c r="E106" s="25" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A107" s="57"/>
+      <c r="A107" s="53"/>
       <c r="E107" s="25" t="s">
         <v>374</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A108" s="57"/>
+      <c r="A108" s="53"/>
       <c r="E108" s="25" t="s">
         <v>375</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A109" s="57"/>
+      <c r="A109" s="53"/>
       <c r="E109" s="25" t="s">
         <v>376</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A110" s="59"/>
+      <c r="A110" s="55"/>
       <c r="D110" s="33"/>
       <c r="E110" s="25" t="s">
         <v>378</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A111" s="56" t="s">
+      <c r="A111" s="52" t="s">
         <v>383</v>
       </c>
       <c r="B111" s="32" t="s">
@@ -5258,7 +5536,7 @@
       </c>
     </row>
     <row r="112" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A112" s="57"/>
+      <c r="A112" s="53"/>
       <c r="B112" s="22" t="s">
         <v>389</v>
       </c>
@@ -5273,7 +5551,7 @@
       </c>
     </row>
     <row r="113" spans="1:5" ht="180" x14ac:dyDescent="0.25">
-      <c r="A113" s="57"/>
+      <c r="A113" s="53"/>
       <c r="B113" s="22" t="s">
         <v>391</v>
       </c>
@@ -5288,7 +5566,7 @@
       </c>
     </row>
     <row r="114" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A114" s="57"/>
+      <c r="A114" s="53"/>
       <c r="B114" s="22" t="s">
         <v>407</v>
       </c>
@@ -5300,7 +5578,7 @@
       </c>
     </row>
     <row r="115" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A115" s="57"/>
+      <c r="A115" s="53"/>
       <c r="B115" s="22" t="s">
         <v>410</v>
       </c>
@@ -5312,7 +5590,7 @@
       </c>
     </row>
     <row r="116" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A116" s="57"/>
+      <c r="A116" s="53"/>
       <c r="B116" s="22" t="s">
         <v>411</v>
       </c>
@@ -5324,7 +5602,7 @@
       </c>
     </row>
     <row r="117" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A117" s="57"/>
+      <c r="A117" s="53"/>
       <c r="C117" s="23" t="s">
         <v>408</v>
       </c>
@@ -5333,7 +5611,7 @@
       </c>
     </row>
     <row r="118" spans="1:5" ht="150" x14ac:dyDescent="0.25">
-      <c r="A118" s="57"/>
+      <c r="A118" s="53"/>
       <c r="C118" s="23" t="s">
         <v>414</v>
       </c>
@@ -5342,7 +5620,7 @@
       </c>
     </row>
     <row r="119" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A119" s="57"/>
+      <c r="A119" s="53"/>
       <c r="C119" s="23" t="s">
         <v>415</v>
       </c>
@@ -5351,37 +5629,37 @@
       </c>
     </row>
     <row r="120" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A120" s="57"/>
+      <c r="A120" s="53"/>
       <c r="E120" s="25" t="s">
         <v>400</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A121" s="57"/>
+      <c r="A121" s="53"/>
       <c r="E121" s="25" t="s">
         <v>401</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="150" x14ac:dyDescent="0.25">
-      <c r="A122" s="57"/>
+      <c r="A122" s="53"/>
       <c r="E122" s="25" t="s">
         <v>402</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A123" s="57"/>
+      <c r="A123" s="53"/>
       <c r="E123" s="25" t="s">
         <v>404</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A124" s="57"/>
+      <c r="A124" s="53"/>
       <c r="E124" s="25" t="s">
         <v>409</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="165" x14ac:dyDescent="0.25">
-      <c r="A125" s="59"/>
+      <c r="A125" s="55"/>
       <c r="B125" s="31"/>
       <c r="C125" s="34"/>
       <c r="D125" s="33"/>
@@ -5390,7 +5668,7 @@
       </c>
     </row>
     <row r="126" spans="1:5" ht="210" x14ac:dyDescent="0.25">
-      <c r="A126" s="56" t="s">
+      <c r="A126" s="52" t="s">
         <v>416</v>
       </c>
       <c r="B126" s="22" t="s">
@@ -5407,7 +5685,7 @@
       </c>
     </row>
     <row r="127" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A127" s="58"/>
+      <c r="A127" s="54"/>
       <c r="B127" s="22" t="s">
         <v>447</v>
       </c>
@@ -5422,7 +5700,7 @@
       </c>
     </row>
     <row r="128" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A128" s="58"/>
+      <c r="A128" s="54"/>
       <c r="B128" s="22" t="s">
         <v>448</v>
       </c>
@@ -5437,7 +5715,7 @@
       </c>
     </row>
     <row r="129" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A129" s="58"/>
+      <c r="A129" s="54"/>
       <c r="B129" s="22" t="s">
         <v>449</v>
       </c>
@@ -5452,7 +5730,7 @@
       </c>
     </row>
     <row r="130" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A130" s="58"/>
+      <c r="A130" s="54"/>
       <c r="C130" s="23" t="s">
         <v>425</v>
       </c>
@@ -5461,7 +5739,7 @@
       </c>
     </row>
     <row r="131" spans="1:5" ht="195" x14ac:dyDescent="0.25">
-      <c r="A131" s="58"/>
+      <c r="A131" s="54"/>
       <c r="C131" s="23" t="s">
         <v>427</v>
       </c>
@@ -5470,7 +5748,7 @@
       </c>
     </row>
     <row r="132" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A132" s="58"/>
+      <c r="A132" s="54"/>
       <c r="C132" s="23" t="s">
         <v>429</v>
       </c>
@@ -5479,7 +5757,7 @@
       </c>
     </row>
     <row r="133" spans="1:5" ht="135" x14ac:dyDescent="0.25">
-      <c r="A133" s="58"/>
+      <c r="A133" s="54"/>
       <c r="C133" s="23" t="s">
         <v>435</v>
       </c>
@@ -5488,7 +5766,7 @@
       </c>
     </row>
     <row r="134" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A134" s="58"/>
+      <c r="A134" s="54"/>
       <c r="C134" s="23" t="s">
         <v>441</v>
       </c>
@@ -5497,7 +5775,7 @@
       </c>
     </row>
     <row r="135" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A135" s="58"/>
+      <c r="A135" s="54"/>
       <c r="C135" s="23" t="s">
         <v>443</v>
       </c>
@@ -5506,7 +5784,7 @@
       </c>
     </row>
     <row r="136" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A136" s="58"/>
+      <c r="A136" s="54"/>
       <c r="C136" s="23" t="s">
         <v>445</v>
       </c>
@@ -5515,8 +5793,8 @@
       </c>
     </row>
     <row r="137" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A137" s="58"/>
-      <c r="C137" s="39" t="s">
+      <c r="A137" s="54"/>
+      <c r="C137" s="38" t="s">
         <v>446</v>
       </c>
       <c r="E137" s="25" t="s">
@@ -5524,136 +5802,136 @@
       </c>
     </row>
     <row r="138" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A138" s="58"/>
-      <c r="C138" s="39"/>
+      <c r="A138" s="54"/>
+      <c r="C138" s="38"/>
       <c r="E138" s="25" t="s">
         <v>444</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A139" s="59"/>
+      <c r="A139" s="55"/>
       <c r="B139" s="31"/>
       <c r="C139" s="34"/>
       <c r="E139" s="27"/>
     </row>
     <row r="140" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A140" s="56" t="s">
-        <v>512</v>
+      <c r="A140" s="52" t="s">
+        <v>510</v>
       </c>
       <c r="B140" s="22" t="s">
+        <v>509</v>
+      </c>
+      <c r="C140" s="23" t="s">
         <v>511</v>
-      </c>
-      <c r="C140" s="23" t="s">
-        <v>513</v>
       </c>
       <c r="D140" s="28"/>
       <c r="E140" s="25" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A141" s="53"/>
+      <c r="B141" s="22" t="s">
+        <v>527</v>
+      </c>
+      <c r="C141" s="23" t="s">
+        <v>513</v>
+      </c>
+      <c r="E141" s="25" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="141" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A141" s="57"/>
-      <c r="B141" s="22" t="s">
+    <row r="142" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A142" s="53"/>
+      <c r="C142" s="23" t="s">
+        <v>516</v>
+      </c>
+      <c r="E142" s="25" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" ht="240" x14ac:dyDescent="0.25">
+      <c r="A143" s="53"/>
+      <c r="C143" s="23" t="s">
         <v>529</v>
       </c>
-      <c r="C141" s="23" t="s">
-        <v>515</v>
-      </c>
-      <c r="E141" s="25" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A142" s="57"/>
-      <c r="C142" s="23" t="s">
+      <c r="E143" s="25" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A144" s="53"/>
+      <c r="C144" s="23" t="s">
+        <v>530</v>
+      </c>
+      <c r="E144" s="25" t="s">
         <v>518</v>
       </c>
-      <c r="E142" s="25" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" ht="240" x14ac:dyDescent="0.25">
-      <c r="A143" s="57"/>
-      <c r="C143" s="23" t="s">
+    </row>
+    <row r="145" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A145" s="53"/>
+      <c r="C145" s="23" t="s">
         <v>531</v>
       </c>
-      <c r="E143" s="25" t="s">
+      <c r="E145" s="25" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A144" s="57"/>
-      <c r="C144" s="23" t="s">
+    <row r="146" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A146" s="53"/>
+      <c r="C146" s="23" t="s">
         <v>532</v>
       </c>
-      <c r="E144" s="25" t="s">
+      <c r="E146" s="25" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="145" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A145" s="57"/>
-      <c r="C145" s="23" t="s">
+    <row r="147" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A147" s="53"/>
+      <c r="E147" s="25" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A148" s="53"/>
+      <c r="E148" s="25" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A149" s="53"/>
+      <c r="E149" s="25" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A150" s="53"/>
+      <c r="E150" s="25" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A151" s="53"/>
+      <c r="E151" s="25" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A152" s="53"/>
+      <c r="E152" s="25" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A153" s="53"/>
+      <c r="E153" s="25" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A154" s="53"/>
+      <c r="E154" s="25" t="s">
         <v>533</v>
-      </c>
-      <c r="E145" s="25" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A146" s="57"/>
-      <c r="C146" s="23" t="s">
-        <v>534</v>
-      </c>
-      <c r="E146" s="25" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A147" s="57"/>
-      <c r="E147" s="25" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A148" s="57"/>
-      <c r="E148" s="25" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A149" s="57"/>
-      <c r="E149" s="25" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A150" s="57"/>
-      <c r="E150" s="25" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" ht="135" x14ac:dyDescent="0.25">
-      <c r="A151" s="57"/>
-      <c r="E151" s="25" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A152" s="57"/>
-      <c r="E152" s="25" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A153" s="57"/>
-      <c r="E153" s="25" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A154" s="57"/>
-      <c r="E154" s="25" t="s">
-        <v>535</v>
       </c>
     </row>
   </sheetData>
@@ -5676,20 +5954,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED5B4F25-E774-4A01-9179-A9A2FE89D1E4}">
-  <dimension ref="A1:L69"/>
+  <dimension ref="A1:L66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G27" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36:K36"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G61" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="21.85546875" customWidth="1"/>
-    <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="12" width="63.42578125" customWidth="1"/>
+    <col min="7" max="7" width="46.5703125" style="59" customWidth="1"/>
+    <col min="8" max="9" width="63.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>452</v>
       </c>
@@ -5703,7 +5981,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>21</v>
       </c>
@@ -5716,11 +5994,8 @@
       <c r="D2" t="s">
         <v>458</v>
       </c>
-      <c r="H2" s="38" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>19</v>
       </c>
@@ -5733,11 +6008,8 @@
       <c r="D3" t="s">
         <v>461</v>
       </c>
-      <c r="H3" s="38" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -5751,7 +6023,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -5765,7 +6037,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -5779,7 +6051,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>8</v>
       </c>
@@ -5793,7 +6065,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>15</v>
       </c>
@@ -5807,7 +6079,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>16</v>
       </c>
@@ -5821,7 +6093,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -5835,7 +6107,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3</v>
       </c>
@@ -5849,7 +6121,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>6</v>
       </c>
@@ -5863,7 +6135,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>18</v>
       </c>
@@ -5877,7 +6149,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>20</v>
       </c>
@@ -5891,7 +6163,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>17</v>
       </c>
@@ -5905,7 +6177,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>7</v>
       </c>
@@ -5919,7 +6191,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>9</v>
       </c>
@@ -5933,7 +6205,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>10</v>
       </c>
@@ -5947,7 +6219,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>11</v>
       </c>
@@ -5961,7 +6233,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>12</v>
       </c>
@@ -5975,7 +6247,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>14</v>
       </c>
@@ -5989,7 +6261,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>13</v>
       </c>
@@ -6003,732 +6275,543 @@
         <v>461</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F25" s="40" t="s">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F25" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="G25" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H25" s="8" t="s">
-        <v>19</v>
+      <c r="G25" s="10" t="s">
+        <v>553</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>2</v>
       </c>
       <c r="I25" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="F26" s="60" t="s">
+        <v>632</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H26" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="F27" s="60"/>
+      <c r="G27" s="4" t="s">
+        <v>554</v>
+      </c>
+      <c r="H27" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="I27" s="4" t="s">
         <v>555</v>
       </c>
-      <c r="J25" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="K25" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="L25" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="F26" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="G26" s="3">
-        <v>2013</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I26" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J26" s="46" t="s">
+    </row>
+    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="F28" s="60"/>
+      <c r="G28" s="4" t="s">
+        <v>556</v>
+      </c>
+      <c r="H28" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="K26" s="4" t="s">
-        <v>554</v>
-      </c>
-      <c r="L26" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="F27" s="60"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4" t="s">
-        <v>556</v>
-      </c>
-      <c r="J27" s="46" t="s">
+      <c r="I28" s="4" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="F29" s="60"/>
+      <c r="G29" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>600</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="F30" s="60"/>
+      <c r="G30" s="4" t="s">
+        <v>559</v>
+      </c>
+      <c r="H30" s="43" t="s">
+        <v>560</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="F31" s="60"/>
+      <c r="G31" s="4" t="s">
+        <v>563</v>
+      </c>
+      <c r="H31" s="43" t="s">
+        <v>589</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="F32" s="60"/>
+      <c r="G32" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H32" s="43" t="s">
+        <v>573</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="33" spans="6:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="F33" s="61" t="s">
+        <v>633</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H33" s="43" t="s">
+        <v>564</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="34" spans="6:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="F34" s="61" t="s">
+        <v>634</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H34" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="K27" s="4" t="s">
-        <v>557</v>
-      </c>
-      <c r="L27" s="3"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F28" s="60"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4" t="s">
-        <v>558</v>
-      </c>
-      <c r="J28" s="46" t="s">
+      <c r="I34" s="4" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="35" spans="6:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F35" s="60" t="s">
+        <v>635</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>567</v>
+      </c>
+      <c r="H35" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="K28" s="4" t="s">
-        <v>559</v>
-      </c>
-      <c r="L28" s="3"/>
-    </row>
-    <row r="29" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="F29" s="60"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4" t="s">
-        <v>565</v>
-      </c>
-      <c r="J29" s="4" t="s">
-        <v>560</v>
-      </c>
-      <c r="K29" s="4" t="s">
-        <v>561</v>
-      </c>
-      <c r="L29" s="3"/>
-    </row>
-    <row r="30" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="F30" s="60"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4" t="s">
+      <c r="I35" s="4" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="36" spans="6:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="F36" s="60"/>
+      <c r="G36" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H36" s="43" t="s">
+        <v>599</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="37" spans="6:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="F37" s="60"/>
+      <c r="G37" s="56" t="s">
+        <v>569</v>
+      </c>
+      <c r="H37" s="57" t="s">
+        <v>588</v>
+      </c>
+      <c r="I37" s="56" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="38" spans="6:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="F38" s="60"/>
+      <c r="G38" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H38" s="43" t="s">
+        <v>573</v>
+      </c>
+      <c r="I38" s="4" t="s">
         <v>562</v>
       </c>
-      <c r="J30" s="46" t="s">
-        <v>563</v>
-      </c>
-      <c r="K30" s="4" t="s">
-        <v>564</v>
-      </c>
-      <c r="L30" s="3"/>
-    </row>
-    <row r="31" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="F31" s="60"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4" t="s">
-        <v>568</v>
-      </c>
-      <c r="J31" s="46" t="s">
+    </row>
+    <row r="39" spans="6:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="F39" s="60"/>
+      <c r="G39" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H39" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="40" spans="6:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="F40" s="60" t="s">
+        <v>636</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>575</v>
+      </c>
+      <c r="H40" s="13" t="s">
+        <v>578</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="41" spans="6:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="F41" s="60"/>
+      <c r="G41" s="4" t="s">
+        <v>574</v>
+      </c>
+      <c r="H41" s="13" t="s">
+        <v>579</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="42" spans="6:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="F42" s="60"/>
+      <c r="G42" s="4" t="s">
+        <v>576</v>
+      </c>
+      <c r="H42" s="13" t="s">
         <v>577</v>
       </c>
-      <c r="K31" s="4" t="s">
-        <v>578</v>
-      </c>
-      <c r="L31" s="3"/>
-    </row>
-    <row r="32" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="F32" s="60"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4" t="s">
+      <c r="I42" s="4" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="43" spans="6:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="F43" s="60"/>
+      <c r="G43" s="4" t="s">
+        <v>586</v>
+      </c>
+      <c r="H43" s="43" t="s">
+        <v>587</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="44" spans="6:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="F44" s="60"/>
+      <c r="G44" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="H44" s="43" t="s">
+        <v>582</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="45" spans="6:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="F45" s="60"/>
+      <c r="G45" s="4" t="s">
+        <v>583</v>
+      </c>
+      <c r="H45" s="43" t="s">
+        <v>584</v>
+      </c>
+      <c r="I45" s="4" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="46" spans="6:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="F46" s="60"/>
+      <c r="G46" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H46" s="43" t="s">
+        <v>590</v>
+      </c>
+      <c r="I46" s="11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="47" spans="6:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F47" s="60" t="s">
+        <v>637</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="H47" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="I47" s="4" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="48" spans="6:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="F48" s="60"/>
+      <c r="G48" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H48" s="43" t="s">
+        <v>622</v>
+      </c>
+      <c r="I48" s="4" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="49" spans="6:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="F49" s="60"/>
+      <c r="G49" s="4" t="s">
+        <v>624</v>
+      </c>
+      <c r="H49" s="43" t="s">
+        <v>626</v>
+      </c>
+      <c r="I49" s="4" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="50" spans="6:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="F50" s="60"/>
+      <c r="G50" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="H50" s="43" t="s">
+        <v>627</v>
+      </c>
+      <c r="I50" s="4" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="51" spans="6:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="F51" s="60"/>
+      <c r="G51" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="H51" s="43" t="s">
+        <v>629</v>
+      </c>
+      <c r="I51" s="4" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="52" spans="6:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="F52" s="60"/>
+      <c r="G52" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H52" s="43" t="s">
+        <v>630</v>
+      </c>
+      <c r="I52" s="4" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="53" spans="6:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="F53" s="60" t="s">
+        <v>638</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H53" s="43" t="s">
+        <v>591</v>
+      </c>
+      <c r="I53" s="4" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="54" spans="6:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="F54" s="60"/>
+      <c r="G54" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H54" s="43" t="s">
+        <v>593</v>
+      </c>
+      <c r="I54" s="4" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="55" spans="6:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="F55" s="60"/>
+      <c r="G55" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H55" s="43" t="s">
+        <v>595</v>
+      </c>
+      <c r="I55" s="4" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="56" spans="6:9" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F56" s="60" t="s">
+        <v>639</v>
+      </c>
+      <c r="G56" s="4" t="s">
+        <v>597</v>
+      </c>
+      <c r="H56" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="I56" s="4" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="57" spans="6:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="F57" s="60"/>
+      <c r="G57" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H57" s="4" t="s">
+        <v>606</v>
+      </c>
+      <c r="I57" s="4" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="58" spans="6:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="F58" s="60"/>
+      <c r="G58" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H58" s="4" t="s">
+        <v>601</v>
+      </c>
+      <c r="I58" s="4" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="59" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F59" s="60"/>
+      <c r="G59" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J32" s="46" t="s">
-        <v>567</v>
-      </c>
-      <c r="K32" s="4" t="s">
-        <v>566</v>
-      </c>
-      <c r="L32" s="3"/>
-    </row>
-    <row r="33" spans="6:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="F33" s="44" t="s">
-        <v>33</v>
-      </c>
-      <c r="G33">
-        <v>2015</v>
-      </c>
-      <c r="H33" s="45" t="s">
-        <v>569</v>
-      </c>
-      <c r="I33" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="J33" s="46" t="s">
-        <v>570</v>
-      </c>
-      <c r="K33" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="L33" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="34" spans="6:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="F34" s="60" t="s">
-        <v>39</v>
-      </c>
-      <c r="G34" s="3">
-        <v>2018</v>
-      </c>
-      <c r="H34" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="I34" s="4" t="s">
-        <v>573</v>
-      </c>
-      <c r="J34" s="46" t="s">
+      <c r="H59" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="K34" s="4" t="s">
-        <v>572</v>
-      </c>
-      <c r="L34" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="35" spans="6:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="F35" s="60"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="J35" s="46" t="s">
-        <v>574</v>
-      </c>
-      <c r="K35" s="4" t="s">
-        <v>575</v>
-      </c>
-      <c r="L35" s="3"/>
-    </row>
-    <row r="36" spans="6:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="F36" s="60"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="62" t="s">
-        <v>576</v>
-      </c>
-      <c r="J36" s="63" t="s">
-        <v>579</v>
-      </c>
-      <c r="K36" s="62" t="s">
-        <v>580</v>
-      </c>
-      <c r="L36" s="3"/>
-    </row>
-    <row r="37" spans="6:12" ht="105" x14ac:dyDescent="0.25">
-      <c r="F37" s="60"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4" t="s">
+      <c r="I59" s="4" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="60" spans="6:9" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F60" s="60" t="s">
+        <v>640</v>
+      </c>
+      <c r="G60" s="43" t="s">
+        <v>91</v>
+      </c>
+      <c r="H60" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I60" s="4" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="61" spans="6:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="F61" s="60"/>
+      <c r="G61" s="43" t="s">
+        <v>93</v>
+      </c>
+      <c r="H61" s="4" t="s">
+        <v>607</v>
+      </c>
+      <c r="I61" s="4" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="62" spans="6:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="F62" s="60"/>
+      <c r="G62" s="43" t="s">
+        <v>95</v>
+      </c>
+      <c r="H62" s="4" t="s">
+        <v>611</v>
+      </c>
+      <c r="I62" s="4" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="63" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F63" s="60"/>
+      <c r="G63" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="J37" s="46" t="s">
-        <v>27</v>
-      </c>
-      <c r="K37" s="4"/>
-      <c r="L37" s="3"/>
-    </row>
-    <row r="38" spans="6:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="F38" s="60"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="4"/>
-      <c r="I38" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="J38" s="46" t="s">
+      <c r="H63" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="K38" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="L38" s="3"/>
-    </row>
-    <row r="39" spans="6:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="F39" s="44" t="s">
-        <v>56</v>
-      </c>
-      <c r="G39">
-        <v>2018</v>
-      </c>
-      <c r="H39" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="I39" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="J39" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="K39" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="L39" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="40" spans="6:12" ht="120" x14ac:dyDescent="0.25">
-      <c r="F40" s="60" t="s">
-        <v>62</v>
-      </c>
-      <c r="G40" s="3">
-        <v>2019</v>
-      </c>
-      <c r="H40" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="I40" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="J40" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="K40" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="L40" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="41" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F41" s="60"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="4"/>
-      <c r="I41" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="J41" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="K41" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="L41" s="3"/>
-    </row>
-    <row r="42" spans="6:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="F42" s="60"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="4"/>
-      <c r="I42" s="4" t="s">
+      <c r="I63" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="64" spans="6:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="F64" s="60" t="s">
+        <v>641</v>
+      </c>
+      <c r="G64" s="4" t="s">
+        <v>614</v>
+      </c>
+      <c r="H64" s="11" t="s">
+        <v>616</v>
+      </c>
+      <c r="I64" s="4" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="65" spans="6:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="F65" s="60"/>
+      <c r="G65" s="4" t="s">
+        <v>617</v>
+      </c>
+      <c r="H65" s="43" t="s">
+        <v>618</v>
+      </c>
+      <c r="I65" s="11" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="66" spans="6:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="F66" s="60"/>
+      <c r="G66" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="J42" s="46" t="s">
-        <v>123</v>
-      </c>
-      <c r="K42" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="L42" s="3"/>
-    </row>
-    <row r="43" spans="6:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="F43" s="60"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="4"/>
-      <c r="I43" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="J43" s="46" t="s">
-        <v>271</v>
-      </c>
-      <c r="K43" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="L43" s="3"/>
-    </row>
-    <row r="44" spans="6:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="F44" s="60"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="4"/>
-      <c r="I44" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="J44" s="46" t="s">
-        <v>125</v>
-      </c>
-      <c r="K44" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="L44" s="3"/>
-    </row>
-    <row r="45" spans="6:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="F45" s="60" t="s">
-        <v>79</v>
-      </c>
-      <c r="G45" s="61">
-        <v>2021</v>
-      </c>
-      <c r="H45" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="I45" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="J45" s="46" t="s">
-        <v>71</v>
-      </c>
-      <c r="K45" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="L45" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="46" spans="6:12" ht="135" x14ac:dyDescent="0.25">
-      <c r="F46" s="60"/>
-      <c r="G46" s="61"/>
-      <c r="H46" s="4"/>
-      <c r="I46" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="J46" s="46" t="s">
-        <v>72</v>
-      </c>
-      <c r="K46" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="L46" s="4"/>
-    </row>
-    <row r="47" spans="6:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="F47" s="60"/>
-      <c r="G47" s="61"/>
-      <c r="H47" s="4"/>
-      <c r="I47" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="J47" s="46" t="s">
-        <v>75</v>
-      </c>
-      <c r="K47" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="L47" s="4"/>
-    </row>
-    <row r="48" spans="6:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="F48" s="60" t="s">
-        <v>78</v>
-      </c>
-      <c r="G48">
-        <v>2022</v>
-      </c>
-      <c r="H48" s="45" t="s">
-        <v>80</v>
-      </c>
-      <c r="I48" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="J48" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="K48" s="4"/>
-      <c r="L48" s="3"/>
-    </row>
-    <row r="49" spans="6:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="F49" s="60"/>
-      <c r="H49" s="45"/>
-      <c r="I49" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="J49" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="K49" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="L49" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="50" spans="6:12" ht="105" x14ac:dyDescent="0.25">
-      <c r="F50" s="60"/>
-      <c r="H50" s="45"/>
-      <c r="I50" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="J50" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="K50" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="L50" s="3"/>
-    </row>
-    <row r="51" spans="6:12" ht="111" x14ac:dyDescent="0.25">
-      <c r="F51" s="60"/>
-      <c r="H51" s="45"/>
-      <c r="I51" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="J51" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="K51" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="L51" s="3"/>
-    </row>
-    <row r="52" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F52" s="60"/>
-      <c r="H52" s="45"/>
-      <c r="I52" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J52" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="K52" s="4"/>
-      <c r="L52" s="3"/>
-    </row>
-    <row r="53" spans="6:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="F53" s="60" t="s">
-        <v>39</v>
-      </c>
-      <c r="G53">
-        <v>2023</v>
-      </c>
-      <c r="H53" s="45" t="s">
-        <v>90</v>
-      </c>
-      <c r="I53" s="46" t="s">
-        <v>91</v>
-      </c>
-      <c r="J53" s="4"/>
-      <c r="K53" s="4"/>
-      <c r="L53" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="54" spans="6:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="F54" s="60"/>
-      <c r="H54" s="45"/>
-      <c r="I54" s="46" t="s">
-        <v>92</v>
-      </c>
-      <c r="J54" s="46"/>
-      <c r="K54" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="L54" s="3"/>
-    </row>
-    <row r="55" spans="6:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="F55" s="60"/>
-      <c r="H55" s="45"/>
-      <c r="I55" s="46" t="s">
-        <v>93</v>
-      </c>
-      <c r="J55" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="K55" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="L55" s="3"/>
-    </row>
-    <row r="56" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F56" s="60"/>
-      <c r="H56" s="45"/>
-      <c r="I56" s="46" t="s">
-        <v>94</v>
-      </c>
-      <c r="J56" s="4"/>
-      <c r="K56" s="4"/>
-      <c r="L56" s="3"/>
-    </row>
-    <row r="57" spans="6:12" ht="105" x14ac:dyDescent="0.25">
-      <c r="F57" s="60"/>
-      <c r="H57" s="45"/>
-      <c r="I57" s="46" t="s">
-        <v>95</v>
-      </c>
-      <c r="J57" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="K57" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="L57" s="3"/>
-    </row>
-    <row r="58" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F58" s="60"/>
-      <c r="H58" s="45"/>
-      <c r="I58" s="46" t="s">
-        <v>16</v>
-      </c>
-      <c r="J58" s="4"/>
-      <c r="K58" s="4"/>
-      <c r="L58" s="3"/>
-    </row>
-    <row r="59" spans="6:12" ht="93" x14ac:dyDescent="0.25">
-      <c r="F59" s="47" t="s">
-        <v>102</v>
-      </c>
-      <c r="G59">
-        <v>2023</v>
-      </c>
-      <c r="H59" s="45" t="s">
-        <v>103</v>
-      </c>
-      <c r="I59" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="J59" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="K59" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="L59" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="60" spans="6:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="F60" s="60"/>
-      <c r="H60" s="45"/>
-      <c r="I60" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="J60" s="46" t="s">
-        <v>112</v>
-      </c>
-      <c r="K60" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="L60" s="3"/>
-    </row>
-    <row r="61" spans="6:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="F61" s="60"/>
-      <c r="H61" s="45"/>
-      <c r="I61" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="J61" s="46" t="s">
-        <v>108</v>
-      </c>
-      <c r="K61" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="L61" s="3"/>
-    </row>
-    <row r="62" spans="6:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="F62" s="60"/>
-      <c r="H62" s="45"/>
-      <c r="I62" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="J62" s="46" t="s">
-        <v>109</v>
-      </c>
-      <c r="K62" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="L62" s="3"/>
-    </row>
-    <row r="63" spans="6:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="F63" s="47" t="s">
-        <v>280</v>
-      </c>
-      <c r="G63">
-        <v>2020</v>
-      </c>
-      <c r="H63" s="45" t="s">
-        <v>283</v>
-      </c>
-      <c r="I63" s="4" t="s">
-        <v>290</v>
-      </c>
-      <c r="J63" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="K63" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="L63" s="3" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="64" spans="6:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="F64" s="60"/>
-      <c r="H64" s="45"/>
-      <c r="I64" s="4" t="s">
-        <v>292</v>
-      </c>
-      <c r="J64" s="46" t="s">
-        <v>293</v>
-      </c>
-      <c r="K64" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="L64" s="3"/>
-    </row>
-    <row r="65" spans="6:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="F65" s="60"/>
-      <c r="H65" s="45"/>
-      <c r="I65" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="J65" s="46" t="s">
-        <v>307</v>
-      </c>
-      <c r="K65" s="4" t="s">
-        <v>310</v>
-      </c>
-      <c r="L65" s="3"/>
-    </row>
-    <row r="66" spans="6:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="F66" s="60"/>
-      <c r="H66" s="45"/>
-      <c r="I66" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="J66" s="46" t="s">
-        <v>308</v>
-      </c>
-      <c r="K66" s="4" t="s">
-        <v>309</v>
-      </c>
-      <c r="L66" s="3"/>
-    </row>
-    <row r="67" spans="6:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="F67" s="60"/>
-      <c r="H67" s="45"/>
-      <c r="I67" s="4" t="s">
-        <v>285</v>
-      </c>
-      <c r="J67" s="46" t="s">
-        <v>333</v>
-      </c>
-      <c r="K67" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="L67" s="3"/>
-    </row>
-    <row r="68" spans="6:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="F68" s="60"/>
-      <c r="H68" s="45"/>
-      <c r="I68" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="J68" s="46" t="s">
-        <v>331</v>
-      </c>
-      <c r="K68" s="4" t="s">
-        <v>336</v>
-      </c>
-      <c r="L68" s="3"/>
-    </row>
-    <row r="69" spans="6:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="F69" s="60"/>
-      <c r="H69" s="45"/>
-      <c r="I69" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="J69" s="46" t="s">
-        <v>332</v>
-      </c>
-      <c r="K69" s="4" t="s">
-        <v>335</v>
-      </c>
-      <c r="L69" s="3"/>
+      <c r="H66" s="43" t="s">
+        <v>620</v>
+      </c>
+      <c r="I66" s="11" t="s">
+        <v>621</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="F47:F52"/>
+    <mergeCell ref="F53:F55"/>
+    <mergeCell ref="F56:F59"/>
+    <mergeCell ref="F60:F63"/>
+    <mergeCell ref="F64:F66"/>
+    <mergeCell ref="F26:F32"/>
+    <mergeCell ref="F35:F39"/>
+    <mergeCell ref="F40:F46"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>